<commit_message>
updated mapping sheet with nodes need to be removed
</commit_message>
<xml_diff>
--- a/schemas/PretrialServices_iepd/artifacts/PretrialAssessment_MappingSpreadsheet.xlsx
+++ b/schemas/PretrialServices_iepd/artifacts/PretrialAssessment_MappingSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buddi/Desktop/PretrialAssessment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\Documents\IEPD\JTMP-Data-Exchange-Specs\schemas\PretrialServices_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="13_ncr:1_{F183E3B0-2370-114A-B65E-9E7EA1294BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66C2FC39-3DAF-4CFC-BC60-64BC8EBF5F49}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F30F92A-E04A-4D28-9A61-38525F0A27B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="781" firstSheet="10" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="781" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="610">
   <si>
     <t xml:space="preserve">Template last updated: </t>
   </si>
@@ -2732,9 +2732,6 @@
     <t xml:space="preserve">Literal </t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>Changes to be made</t>
   </si>
   <si>
@@ -2745,6 +2742,18 @@
   </si>
   <si>
     <t>Delete every element other than nc:EntityPerson/nc:PersonName/nc:PersonFullName within nc:AssessmentAssessor</t>
+  </si>
+  <si>
+    <t>AssessmentPerson</t>
+  </si>
+  <si>
+    <t>Uncomment nc:Date and delete nc:DateTime within nc:PersonBirthDate</t>
+  </si>
+  <si>
+    <t>Delete every element other than nc:EntityPerson/nc:PersonName/nc:PersonFullName within nc:DocumentAuthor</t>
+  </si>
+  <si>
+    <t>Delete every element other than nc:EntityPerson/nc:PersonName/nc:PersonFullName within nc:DocumentContributor</t>
   </si>
 </sst>
 </file>
@@ -3005,13 +3014,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -3025,6 +3027,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -3086,7 +3096,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3171,6 +3181,58 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -3179,24 +3241,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -3273,7 +3324,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3567,27 +3618,31 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="35" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -5365,14 +5420,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="28.453125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="51.453125" style="17" customWidth="1"/>
     <col min="3" max="4" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.95">
+    <row r="1" spans="1:4">
       <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
@@ -5394,7 +5449,7 @@
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
     </row>
-    <row r="5" spans="1:4" ht="32.1">
+    <row r="5" spans="1:4" ht="29">
       <c r="A5" s="29" t="s">
         <v>3</v>
       </c>
@@ -5408,7 +5463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.95">
+    <row r="6" spans="1:4">
       <c r="A6" s="30" t="s">
         <v>7</v>
       </c>
@@ -5422,7 +5477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.95">
+    <row r="7" spans="1:4">
       <c r="A7" s="30" t="s">
         <v>11</v>
       </c>
@@ -5436,7 +5491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.95">
+    <row r="8" spans="1:4">
       <c r="A8" s="30" t="s">
         <v>15</v>
       </c>
@@ -5450,7 +5505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.95">
+    <row r="9" spans="1:4">
       <c r="A9" s="30" t="s">
         <v>18</v>
       </c>
@@ -5464,7 +5519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32.1">
+    <row r="10" spans="1:4" ht="29">
       <c r="A10" s="30" t="s">
         <v>21</v>
       </c>
@@ -5478,7 +5533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.95">
+    <row r="11" spans="1:4">
       <c r="A11" s="30" t="s">
         <v>24</v>
       </c>
@@ -5492,7 +5547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.95">
+    <row r="12" spans="1:4">
       <c r="A12" s="30" t="s">
         <v>27</v>
       </c>
@@ -5506,7 +5561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.95">
+    <row r="13" spans="1:4">
       <c r="A13" s="30" t="s">
         <v>31</v>
       </c>
@@ -5528,7 +5583,7 @@
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
     </row>
-    <row r="16" spans="1:4" ht="15.95">
+    <row r="16" spans="1:4">
       <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
@@ -5537,7 +5592,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32.1">
+    <row r="18" spans="1:4" ht="29">
       <c r="A18" s="29" t="s">
         <v>36</v>
       </c>
@@ -5551,7 +5606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="48">
+    <row r="19" spans="1:4" ht="43.5">
       <c r="A19" s="31" t="s">
         <v>37</v>
       </c>
@@ -5565,7 +5620,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48">
+    <row r="20" spans="1:4" ht="43.5">
       <c r="A20" s="31" t="s">
         <v>41</v>
       </c>
@@ -5579,7 +5634,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="48">
+    <row r="21" spans="1:4" ht="43.5">
       <c r="A21" s="31" t="s">
         <v>45</v>
       </c>
@@ -5593,7 +5648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="32.1">
+    <row r="22" spans="1:4" ht="29">
       <c r="A22" s="31" t="s">
         <v>49</v>
       </c>
@@ -5607,7 +5662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32.1">
+    <row r="23" spans="1:4" ht="29">
       <c r="A23" s="31" t="s">
         <v>52</v>
       </c>
@@ -5621,7 +5676,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="48">
+    <row r="24" spans="1:4" ht="43.5">
       <c r="A24" s="31" t="s">
         <v>56</v>
       </c>
@@ -5635,7 +5690,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="48">
+    <row r="25" spans="1:4" ht="43.5">
       <c r="A25" s="31" t="s">
         <v>60</v>
       </c>
@@ -5649,7 +5704,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48">
+    <row r="26" spans="1:4" ht="43.5">
       <c r="A26" s="31" t="s">
         <v>63</v>
       </c>
@@ -5663,7 +5718,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="96">
+    <row r="27" spans="1:4" ht="87">
       <c r="A27" s="31" t="s">
         <v>67</v>
       </c>
@@ -5677,7 +5732,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="48">
+    <row r="28" spans="1:4" ht="43.5">
       <c r="A28" s="31" t="s">
         <v>71</v>
       </c>
@@ -5691,7 +5746,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.95">
+    <row r="31" spans="1:4">
       <c r="A31" s="29" t="s">
         <v>75</v>
       </c>
@@ -5699,7 +5754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="80.099999999999994">
+    <row r="32" spans="1:4" ht="72.5">
       <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
@@ -5707,7 +5762,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="48">
+    <row r="33" spans="1:2" ht="58">
       <c r="A33" s="5" t="s">
         <v>78</v>
       </c>
@@ -5715,7 +5770,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="48">
+    <row r="34" spans="1:2" ht="43.5">
       <c r="A34" s="5" t="s">
         <v>80</v>
       </c>
@@ -5723,7 +5778,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="32.1">
+    <row r="35" spans="1:2" ht="29">
       <c r="A35" s="5" t="s">
         <v>82</v>
       </c>
@@ -5731,7 +5786,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="48">
+    <row r="36" spans="1:2" ht="43.5">
       <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
@@ -5739,7 +5794,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="32.1">
+    <row r="37" spans="1:2" ht="29">
       <c r="A37" s="5" t="s">
         <v>86</v>
       </c>
@@ -5747,7 +5802,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="32.1">
+    <row r="38" spans="1:2" ht="29">
       <c r="A38" s="5" t="s">
         <v>88</v>
       </c>
@@ -5755,7 +5810,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="111.95">
+    <row r="39" spans="1:2" ht="101.5">
       <c r="A39" s="30" t="s">
         <v>90</v>
       </c>
@@ -5763,7 +5818,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="80.099999999999994">
+    <row r="40" spans="1:2" ht="72.5">
       <c r="A40" s="30" t="s">
         <v>92</v>
       </c>
@@ -5790,21 +5845,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
-    <col min="2" max="4" width="20.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="17" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="15.453125" style="2" customWidth="1"/>
+    <col min="2" max="4" width="20.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" style="17" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.81640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="30.453125" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.1">
+    <row r="1" spans="1:11" ht="29">
       <c r="A1" s="10" t="s">
         <v>599</v>
       </c>
@@ -5856,58 +5911,84 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09323929-BD78-4E6B-8E56-D5174B7ABCAB}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="174.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
+    <col min="2" max="2" width="174.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="120"/>
+      <c r="B1" s="121" t="s">
         <v>602</v>
       </c>
-      <c r="B1" s="118" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A2" s="124" t="s">
+        <v>386</v>
+      </c>
+      <c r="B2" s="122" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A2" s="121" t="s">
-        <v>386</v>
-      </c>
-      <c r="B2" s="119" t="s">
+    <row r="3" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A3" s="125"/>
+      <c r="B3" s="123"/>
+    </row>
+    <row r="4" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A4" s="124" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A3" s="122"/>
-      <c r="B3" s="120" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A4" s="121" t="s">
+      <c r="B4" s="123" t="s">
         <v>605</v>
       </c>
-      <c r="B4" s="120" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A5" s="125"/>
+      <c r="B5" s="123"/>
+    </row>
+    <row r="6" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A6" s="127" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A5" s="122"/>
-      <c r="B5" s="120" t="s">
-        <v>602</v>
-      </c>
+      <c r="B6" s="122" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A7" s="128"/>
+      <c r="B7" s="126"/>
+    </row>
+    <row r="8" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A8" s="127" t="s">
+        <v>505</v>
+      </c>
+      <c r="B8" s="123" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A9" s="129"/>
+      <c r="B9" s="123" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.5" customHeight="1">
+      <c r="A10" s="128"/>
+      <c r="B10" s="123"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5921,13 +6002,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28.453125" style="17" customWidth="1"/>
     <col min="3" max="3" width="76" style="17" customWidth="1"/>
-    <col min="4" max="5" width="29.42578125" style="16" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="16"/>
+    <col min="4" max="5" width="29.453125" style="16" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -5944,7 +6025,7 @@
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
     </row>
-    <row r="5" spans="1:3" ht="15.95">
+    <row r="5" spans="1:3">
       <c r="A5" s="68"/>
       <c r="B5" s="69" t="s">
         <v>96</v>
@@ -5953,7 +6034,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.95">
+    <row r="6" spans="1:3">
       <c r="A6" s="68"/>
       <c r="B6" s="69" t="s">
         <v>98</v>
@@ -5962,7 +6043,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.95">
+    <row r="7" spans="1:3">
       <c r="A7" s="68"/>
       <c r="B7" s="69" t="s">
         <v>100</v>
@@ -5971,7 +6052,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.95">
+    <row r="8" spans="1:3">
       <c r="A8" s="68"/>
       <c r="B8" s="69" t="s">
         <v>4</v>
@@ -5980,7 +6061,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.95">
+    <row r="9" spans="1:3">
       <c r="A9" s="68"/>
       <c r="B9" s="69" t="s">
         <v>103</v>
@@ -5989,7 +6070,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="32.1">
+    <row r="10" spans="1:3" ht="29">
       <c r="A10" s="68"/>
       <c r="B10" s="69" t="s">
         <v>105</v>
@@ -5998,7 +6079,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.95">
+    <row r="11" spans="1:3">
       <c r="A11" s="68"/>
       <c r="B11" s="69" t="s">
         <v>107</v>
@@ -6014,7 +6095,7 @@
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
     </row>
-    <row r="13" spans="1:3" ht="15.95">
+    <row r="13" spans="1:3">
       <c r="A13" s="68"/>
       <c r="B13" s="69" t="s">
         <v>110</v>
@@ -6030,7 +6111,7 @@
       </c>
       <c r="C14" s="33"/>
     </row>
-    <row r="15" spans="1:3" ht="15.95">
+    <row r="15" spans="1:3">
       <c r="A15" s="68"/>
       <c r="B15" s="70" t="s">
         <v>113</v>
@@ -6039,7 +6120,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="32.1">
+    <row r="16" spans="1:3" ht="29">
       <c r="A16" s="68"/>
       <c r="B16" s="70" t="s">
         <v>115</v>
@@ -6048,7 +6129,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.95">
+    <row r="17" spans="1:3">
       <c r="A17" s="68"/>
       <c r="B17" s="70" t="s">
         <v>117</v>
@@ -6057,7 +6138,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="32.1">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="68"/>
       <c r="B18" s="70" t="s">
         <v>119</v>
@@ -6066,7 +6147,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.95">
+    <row r="19" spans="1:3">
       <c r="A19" s="68"/>
       <c r="B19" s="70" t="s">
         <v>121</v>
@@ -6075,7 +6156,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.95">
+    <row r="20" spans="1:3">
       <c r="A20" s="68"/>
       <c r="B20" s="70" t="s">
         <v>71</v>
@@ -6084,7 +6165,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.95">
+    <row r="21" spans="1:3">
       <c r="A21" s="68"/>
       <c r="B21" s="70" t="s">
         <v>124</v>
@@ -6100,7 +6181,7 @@
       </c>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="1:3" ht="15.95">
+    <row r="23" spans="1:3">
       <c r="A23" s="68"/>
       <c r="B23" s="69" t="s">
         <v>4</v>
@@ -6109,7 +6190,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.95">
+    <row r="24" spans="1:3">
       <c r="A24" s="68"/>
       <c r="B24" s="69" t="s">
         <v>128</v>
@@ -6118,7 +6199,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.95">
+    <row r="25" spans="1:3">
       <c r="A25" s="68"/>
       <c r="B25" s="69" t="s">
         <v>107</v>
@@ -6134,7 +6215,7 @@
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="1:3" ht="15.95">
+    <row r="27" spans="1:3">
       <c r="A27" s="68"/>
       <c r="B27" s="69" t="s">
         <v>132</v>
@@ -6143,7 +6224,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.95">
+    <row r="28" spans="1:3">
       <c r="A28" s="68"/>
       <c r="B28" s="69" t="s">
         <v>4</v>
@@ -6152,7 +6233,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="32.1">
+    <row r="29" spans="1:3" ht="29">
       <c r="A29" s="68"/>
       <c r="B29" s="69" t="s">
         <v>10</v>
@@ -6161,7 +6242,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.95">
+    <row r="30" spans="1:3">
       <c r="A30" s="68"/>
       <c r="B30" s="69" t="s">
         <v>103</v>
@@ -6170,7 +6251,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="32.1">
+    <row r="31" spans="1:3" ht="29">
       <c r="A31" s="68"/>
       <c r="B31" s="69" t="s">
         <v>105</v>
@@ -6179,7 +6260,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.95">
+    <row r="32" spans="1:3">
       <c r="A32" s="68"/>
       <c r="B32" s="69" t="s">
         <v>107</v>
@@ -6206,7 +6287,7 @@
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
     </row>
-    <row r="37" spans="1:3" ht="15.95">
+    <row r="37" spans="1:3">
       <c r="A37" s="39"/>
       <c r="B37" s="32" t="s">
         <v>141</v>
@@ -6215,7 +6296,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.95">
+    <row r="38" spans="1:3">
       <c r="A38" s="39"/>
       <c r="B38" s="32" t="s">
         <v>143</v>
@@ -6224,7 +6305,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.95">
+    <row r="39" spans="1:3">
       <c r="A39" s="39"/>
       <c r="B39" s="32" t="s">
         <v>145</v>
@@ -6233,7 +6314,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.95">
+    <row r="40" spans="1:3">
       <c r="A40" s="39"/>
       <c r="B40" s="32" t="s">
         <v>147</v>
@@ -6249,7 +6330,7 @@
       <c r="B41" s="50"/>
       <c r="C41" s="50"/>
     </row>
-    <row r="42" spans="1:3" ht="15.95">
+    <row r="42" spans="1:3">
       <c r="A42" s="40"/>
       <c r="B42" s="33" t="s">
         <v>149</v>
@@ -6265,7 +6346,7 @@
       <c r="B43" s="41"/>
       <c r="C43" s="41"/>
     </row>
-    <row r="44" spans="1:3" ht="15.95">
+    <row r="44" spans="1:3">
       <c r="A44" s="42"/>
       <c r="B44" s="32" t="s">
         <v>141</v>
@@ -6274,7 +6355,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.95">
+    <row r="45" spans="1:3">
       <c r="A45" s="42"/>
       <c r="B45" s="32" t="s">
         <v>143</v>
@@ -6283,7 +6364,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="32.1">
+    <row r="46" spans="1:3" ht="29">
       <c r="A46" s="42"/>
       <c r="B46" s="32" t="s">
         <v>152</v>
@@ -6292,7 +6373,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.95">
+    <row r="47" spans="1:3">
       <c r="A47" s="42"/>
       <c r="B47" s="32" t="s">
         <v>147</v>
@@ -6301,7 +6382,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="48">
+    <row r="48" spans="1:3" ht="58">
       <c r="A48" s="42"/>
       <c r="B48" s="32" t="s">
         <v>154</v>
@@ -6310,14 +6391,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.95">
+    <row r="49" spans="1:3">
       <c r="A49" s="42"/>
       <c r="B49" s="32" t="s">
         <v>156</v>
       </c>
       <c r="C49" s="43"/>
     </row>
-    <row r="50" spans="1:3" ht="32.1">
+    <row r="50" spans="1:3" ht="29">
       <c r="A50" s="42"/>
       <c r="B50" s="49" t="s">
         <v>157</v>
@@ -6326,7 +6407,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.95">
+    <row r="51" spans="1:3">
       <c r="A51" s="42"/>
       <c r="B51" s="49" t="s">
         <v>159</v>
@@ -6335,7 +6416,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.95">
+    <row r="52" spans="1:3">
       <c r="A52" s="42"/>
       <c r="B52" s="49" t="s">
         <v>161</v>
@@ -6344,7 +6425,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="32.1">
+    <row r="53" spans="1:3" ht="29">
       <c r="A53" s="42"/>
       <c r="B53" s="32" t="s">
         <v>163</v>
@@ -6353,7 +6434,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.95">
+    <row r="54" spans="1:3">
       <c r="A54" s="42"/>
       <c r="B54" s="32" t="s">
         <v>165</v>
@@ -6362,7 +6443,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.95">
+    <row r="55" spans="1:3">
       <c r="A55" s="42"/>
       <c r="B55" s="32" t="s">
         <v>167</v>
@@ -6378,7 +6459,7 @@
       <c r="B56" s="52"/>
       <c r="C56" s="52"/>
     </row>
-    <row r="57" spans="1:3" ht="15.95">
+    <row r="57" spans="1:3">
       <c r="A57" s="8"/>
       <c r="B57" s="7" t="s">
         <v>170</v>
@@ -6387,7 +6468,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="32.1">
+    <row r="58" spans="1:3" ht="29">
       <c r="A58" s="8"/>
       <c r="B58" s="7" t="s">
         <v>172</v>
@@ -6396,7 +6477,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="32.1">
+    <row r="59" spans="1:3" ht="29">
       <c r="A59" s="8"/>
       <c r="B59" s="7" t="s">
         <v>174</v>
@@ -6405,7 +6486,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="32.1">
+    <row r="60" spans="1:3" ht="29">
       <c r="A60" s="8"/>
       <c r="B60" s="7" t="s">
         <v>176</v>
@@ -6414,7 +6495,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="32.1">
+    <row r="61" spans="1:3" ht="29">
       <c r="A61" s="8"/>
       <c r="B61" s="7" t="s">
         <v>178</v>
@@ -6452,7 +6533,7 @@
       <c r="B66" s="38"/>
       <c r="C66" s="38"/>
     </row>
-    <row r="67" spans="1:3" ht="15.95">
+    <row r="67" spans="1:3">
       <c r="A67" s="39"/>
       <c r="B67" s="32" t="s">
         <v>181</v>
@@ -6461,7 +6542,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.95">
+    <row r="68" spans="1:3">
       <c r="A68" s="39"/>
       <c r="B68" s="32" t="s">
         <v>183</v>
@@ -6470,7 +6551,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.95">
+    <row r="69" spans="1:3">
       <c r="A69" s="39"/>
       <c r="B69" s="32" t="s">
         <v>185</v>
@@ -6479,7 +6560,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.95">
+    <row r="70" spans="1:3">
       <c r="A70" s="39"/>
       <c r="B70" s="32" t="s">
         <v>147</v>
@@ -6495,7 +6576,7 @@
       <c r="B71" s="50"/>
       <c r="C71" s="50"/>
     </row>
-    <row r="72" spans="1:3" ht="15.95">
+    <row r="72" spans="1:3">
       <c r="A72" s="40"/>
       <c r="B72" s="33" t="s">
         <v>149</v>
@@ -6511,7 +6592,7 @@
       <c r="B73" s="41"/>
       <c r="C73" s="41"/>
     </row>
-    <row r="74" spans="1:3" ht="15.95">
+    <row r="74" spans="1:3">
       <c r="A74" s="40"/>
       <c r="B74" s="32" t="s">
         <v>181</v>
@@ -6520,7 +6601,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.95">
+    <row r="75" spans="1:3">
       <c r="A75" s="40"/>
       <c r="B75" s="32" t="s">
         <v>183</v>
@@ -6529,7 +6610,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.95">
+    <row r="76" spans="1:3">
       <c r="A76" s="40"/>
       <c r="B76" s="32" t="s">
         <v>147</v>
@@ -6538,7 +6619,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.95">
+    <row r="77" spans="1:3">
       <c r="A77" s="40"/>
       <c r="B77" s="32" t="s">
         <v>185</v>
@@ -6547,14 +6628,14 @@
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.95">
+    <row r="78" spans="1:3">
       <c r="A78" s="40"/>
       <c r="B78" s="32" t="s">
         <v>188</v>
       </c>
       <c r="C78" s="32"/>
     </row>
-    <row r="79" spans="1:3" ht="15.95">
+    <row r="79" spans="1:3">
       <c r="A79" s="40"/>
       <c r="B79" s="49" t="s">
         <v>189</v>
@@ -6563,7 +6644,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.95">
+    <row r="80" spans="1:3">
       <c r="A80" s="40"/>
       <c r="B80" s="49" t="s">
         <v>191</v>
@@ -6572,7 +6653,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="32.1">
+    <row r="81" spans="1:3" ht="29">
       <c r="A81" s="40"/>
       <c r="B81" s="49" t="s">
         <v>193</v>
@@ -6581,7 +6662,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.95">
+    <row r="82" spans="1:3">
       <c r="A82" s="40"/>
       <c r="B82" s="49" t="s">
         <v>195</v>
@@ -6590,7 +6671,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.95">
+    <row r="83" spans="1:3">
       <c r="A83" s="40"/>
       <c r="B83" s="49" t="s">
         <v>197</v>
@@ -6599,7 +6680,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.95">
+    <row r="84" spans="1:3">
       <c r="A84" s="40"/>
       <c r="B84" s="49" t="s">
         <v>199</v>
@@ -6608,7 +6689,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.95">
+    <row r="85" spans="1:3">
       <c r="A85" s="40"/>
       <c r="B85" s="49" t="s">
         <v>201</v>
@@ -6617,7 +6698,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="32.1">
+    <row r="86" spans="1:3" ht="29">
       <c r="A86" s="40"/>
       <c r="B86" s="49" t="s">
         <v>203</v>
@@ -6626,7 +6707,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="32.1">
+    <row r="87" spans="1:3" ht="29">
       <c r="A87" s="40"/>
       <c r="B87" s="49" t="s">
         <v>205</v>
@@ -6635,7 +6716,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="32.1">
+    <row r="88" spans="1:3" ht="29">
       <c r="A88" s="40"/>
       <c r="B88" s="32" t="s">
         <v>207</v>
@@ -6644,7 +6725,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="63.95">
+    <row r="89" spans="1:3" ht="72.5">
       <c r="A89" s="40"/>
       <c r="B89" s="32" t="s">
         <v>209</v>
@@ -6653,7 +6734,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="63.95" hidden="1">
+    <row r="90" spans="1:3" ht="72.5" hidden="1">
       <c r="A90" s="40"/>
       <c r="B90" s="32" t="s">
         <v>211</v>
@@ -6669,7 +6750,7 @@
       <c r="B91" s="52"/>
       <c r="C91" s="52"/>
     </row>
-    <row r="92" spans="1:3" ht="15.95">
+    <row r="92" spans="1:3">
       <c r="A92" s="8"/>
       <c r="B92" s="7" t="s">
         <v>170</v>
@@ -6678,7 +6759,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="32.1">
+    <row r="93" spans="1:3" ht="29">
       <c r="A93" s="8"/>
       <c r="B93" s="7" t="s">
         <v>214</v>
@@ -6687,7 +6768,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="32.1">
+    <row r="94" spans="1:3" ht="29">
       <c r="A94" s="8"/>
       <c r="B94" s="7" t="s">
         <v>216</v>
@@ -6725,7 +6806,7 @@
       <c r="B99" s="38"/>
       <c r="C99" s="38"/>
     </row>
-    <row r="100" spans="1:3" ht="15.95">
+    <row r="100" spans="1:3">
       <c r="A100" s="39"/>
       <c r="B100" s="32" t="s">
         <v>219</v>
@@ -6734,7 +6815,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.95">
+    <row r="101" spans="1:3">
       <c r="A101" s="39"/>
       <c r="B101" s="32" t="s">
         <v>183</v>
@@ -6743,7 +6824,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15.95">
+    <row r="102" spans="1:3">
       <c r="A102" s="39"/>
       <c r="B102" s="32" t="s">
         <v>221</v>
@@ -6752,7 +6833,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15.95">
+    <row r="103" spans="1:3">
       <c r="A103" s="39"/>
       <c r="B103" s="32" t="s">
         <v>143</v>
@@ -6761,7 +6842,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.95">
+    <row r="104" spans="1:3">
       <c r="A104" s="39"/>
       <c r="B104" s="32" t="s">
         <v>223</v>
@@ -6770,7 +6851,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="32.1">
+    <row r="105" spans="1:3" ht="29">
       <c r="A105" s="39"/>
       <c r="B105" s="32" t="s">
         <v>225</v>
@@ -6786,7 +6867,7 @@
       <c r="B106" s="50"/>
       <c r="C106" s="50"/>
     </row>
-    <row r="107" spans="1:3" ht="15.95">
+    <row r="107" spans="1:3">
       <c r="A107" s="40"/>
       <c r="B107" s="33" t="s">
         <v>149</v>
@@ -6802,7 +6883,7 @@
       <c r="B108" s="41"/>
       <c r="C108" s="41"/>
     </row>
-    <row r="109" spans="1:3" ht="15.95">
+    <row r="109" spans="1:3">
       <c r="A109" s="39"/>
       <c r="B109" s="32" t="s">
         <v>219</v>
@@ -6811,7 +6892,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15.95">
+    <row r="110" spans="1:3">
       <c r="A110" s="39"/>
       <c r="B110" s="32" t="s">
         <v>183</v>
@@ -6820,7 +6901,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="15.95">
+    <row r="111" spans="1:3">
       <c r="A111" s="39"/>
       <c r="B111" s="32" t="s">
         <v>221</v>
@@ -6829,7 +6910,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="1:3" customFormat="1" ht="15.95">
+    <row r="112" spans="1:3" customFormat="1">
       <c r="A112" s="39"/>
       <c r="B112" s="32" t="s">
         <v>143</v>
@@ -6838,7 +6919,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="113" spans="1:3" customFormat="1" ht="15.95">
+    <row r="113" spans="1:3" customFormat="1">
       <c r="A113" s="39"/>
       <c r="B113" s="32" t="s">
         <v>223</v>
@@ -6847,7 +6928,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="15.95">
+    <row r="114" spans="1:3">
       <c r="A114" s="39"/>
       <c r="B114" s="49" t="s">
         <v>227</v>
@@ -6856,7 +6937,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="15.95">
+    <row r="115" spans="1:3">
       <c r="A115" s="39"/>
       <c r="B115" s="32" t="s">
         <v>225</v>
@@ -6865,7 +6946,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="15.95">
+    <row r="116" spans="1:3">
       <c r="A116" s="39"/>
       <c r="B116" s="49" t="s">
         <v>230</v>
@@ -6874,7 +6955,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="15.95">
+    <row r="117" spans="1:3">
       <c r="A117" s="39"/>
       <c r="B117" s="32" t="s">
         <v>147</v>
@@ -6883,7 +6964,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="15.95">
+    <row r="118" spans="1:3">
       <c r="A118" s="39"/>
       <c r="B118" s="32" t="s">
         <v>233</v>
@@ -6927,7 +7008,7 @@
       <c r="B125" s="38"/>
       <c r="C125" s="38"/>
     </row>
-    <row r="126" spans="1:3" ht="15.95">
+    <row r="126" spans="1:3">
       <c r="A126" s="39"/>
       <c r="B126" s="32" t="s">
         <v>237</v>
@@ -6936,7 +7017,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="15.95">
+    <row r="127" spans="1:3">
       <c r="A127" s="39"/>
       <c r="B127" s="32" t="s">
         <v>183</v>
@@ -6945,7 +7026,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="15.95">
+    <row r="128" spans="1:3">
       <c r="A128" s="39"/>
       <c r="B128" s="32" t="s">
         <v>238</v>
@@ -6954,7 +7035,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.95">
+    <row r="129" spans="1:3">
       <c r="A129" s="39"/>
       <c r="B129" s="32" t="s">
         <v>147</v>
@@ -6970,7 +7051,7 @@
       <c r="B130" s="50"/>
       <c r="C130" s="50"/>
     </row>
-    <row r="131" spans="1:3" ht="15.95">
+    <row r="131" spans="1:3">
       <c r="A131" s="40"/>
       <c r="B131" s="33" t="s">
         <v>149</v>
@@ -6986,7 +7067,7 @@
       <c r="B132" s="41"/>
       <c r="C132" s="41"/>
     </row>
-    <row r="133" spans="1:3" ht="15.95">
+    <row r="133" spans="1:3">
       <c r="A133" s="39"/>
       <c r="B133" s="32" t="s">
         <v>237</v>
@@ -6995,7 +7076,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15.95">
+    <row r="134" spans="1:3">
       <c r="A134" s="39"/>
       <c r="B134" s="32" t="s">
         <v>183</v>
@@ -7004,7 +7085,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15.95">
+    <row r="135" spans="1:3">
       <c r="A135" s="40"/>
       <c r="B135" s="32" t="s">
         <v>238</v>
@@ -7013,7 +7094,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.95">
+    <row r="136" spans="1:3">
       <c r="A136" s="40"/>
       <c r="B136" s="32" t="s">
         <v>147</v>
@@ -7022,7 +7103,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="32.1">
+    <row r="137" spans="1:3" ht="29">
       <c r="A137" s="40"/>
       <c r="B137" s="32" t="s">
         <v>242</v>
@@ -7031,7 +7112,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15.95">
+    <row r="138" spans="1:3">
       <c r="A138" s="40"/>
       <c r="B138" s="49" t="s">
         <v>244</v>
@@ -7040,7 +7121,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15.95">
+    <row r="139" spans="1:3">
       <c r="A139" s="40"/>
       <c r="B139" s="49" t="s">
         <v>246</v>
@@ -7049,7 +7130,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.95">
+    <row r="140" spans="1:3">
       <c r="A140" s="40"/>
       <c r="B140" s="49" t="s">
         <v>248</v>
@@ -7058,7 +7139,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.95">
+    <row r="141" spans="1:3">
       <c r="A141" s="40"/>
       <c r="B141" s="49" t="s">
         <v>250</v>
@@ -7067,7 +7148,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.95">
+    <row r="142" spans="1:3">
       <c r="A142" s="40"/>
       <c r="B142" s="49" t="s">
         <v>252</v>
@@ -7076,7 +7157,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15.95">
+    <row r="143" spans="1:3">
       <c r="A143" s="40"/>
       <c r="B143" s="49" t="s">
         <v>254</v>
@@ -7085,7 +7166,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.95">
+    <row r="144" spans="1:3">
       <c r="A144" s="40"/>
       <c r="B144" s="49" t="s">
         <v>256</v>
@@ -7094,7 +7175,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="15.95">
+    <row r="145" spans="1:3">
       <c r="A145" s="40"/>
       <c r="B145" s="49" t="s">
         <v>258</v>
@@ -7103,7 +7184,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.95">
+    <row r="146" spans="1:3">
       <c r="A146" s="40"/>
       <c r="B146" s="49" t="s">
         <v>260</v>
@@ -7112,7 +7193,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.95">
+    <row r="147" spans="1:3">
       <c r="A147" s="40"/>
       <c r="B147" s="49" t="s">
         <v>262</v>
@@ -7121,7 +7202,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="15.95">
+    <row r="148" spans="1:3">
       <c r="A148" s="40"/>
       <c r="B148" s="49" t="s">
         <v>264</v>
@@ -7130,7 +7211,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.95">
+    <row r="149" spans="1:3">
       <c r="A149" s="40"/>
       <c r="B149" s="49" t="s">
         <v>266</v>
@@ -7184,7 +7265,7 @@
       <c r="B156" s="38"/>
       <c r="C156" s="38"/>
     </row>
-    <row r="157" spans="1:3" ht="15.95">
+    <row r="157" spans="1:3">
       <c r="A157" s="39"/>
       <c r="B157" s="32" t="s">
         <v>237</v>
@@ -7193,7 +7274,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15.95">
+    <row r="158" spans="1:3">
       <c r="A158" s="39"/>
       <c r="B158" s="32" t="s">
         <v>271</v>
@@ -7202,7 +7283,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15.95">
+    <row r="159" spans="1:3">
       <c r="A159" s="39"/>
       <c r="B159" s="32" t="s">
         <v>147</v>
@@ -7218,7 +7299,7 @@
       <c r="B160" s="50"/>
       <c r="C160" s="50"/>
     </row>
-    <row r="161" spans="1:3" ht="15.95">
+    <row r="161" spans="1:3">
       <c r="A161" s="40"/>
       <c r="B161" s="33" t="s">
         <v>149</v>
@@ -7234,7 +7315,7 @@
       <c r="B162" s="41"/>
       <c r="C162" s="41"/>
     </row>
-    <row r="163" spans="1:3" ht="15.95">
+    <row r="163" spans="1:3">
       <c r="A163" s="40"/>
       <c r="B163" s="32" t="s">
         <v>237</v>
@@ -7243,14 +7324,14 @@
         <v>270</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15.95">
+    <row r="164" spans="1:3">
       <c r="A164" s="40"/>
       <c r="B164" s="32" t="s">
         <v>188</v>
       </c>
       <c r="C164" s="32"/>
     </row>
-    <row r="165" spans="1:3" ht="15.95">
+    <row r="165" spans="1:3">
       <c r="A165" s="40"/>
       <c r="B165" s="49" t="s">
         <v>274</v>
@@ -7259,7 +7340,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15.95">
+    <row r="166" spans="1:3">
       <c r="A166" s="40"/>
       <c r="B166" s="49" t="s">
         <v>276</v>
@@ -7268,7 +7349,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.95">
+    <row r="167" spans="1:3">
       <c r="A167" s="40"/>
       <c r="B167" s="49" t="s">
         <v>278</v>
@@ -7277,7 +7358,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.95">
+    <row r="168" spans="1:3">
       <c r="A168" s="40"/>
       <c r="B168" s="49" t="s">
         <v>280</v>
@@ -7286,7 +7367,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.95">
+    <row r="169" spans="1:3">
       <c r="A169" s="40"/>
       <c r="B169" s="49" t="s">
         <v>191</v>
@@ -7295,7 +7376,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="32.1">
+    <row r="170" spans="1:3" ht="29">
       <c r="A170" s="40"/>
       <c r="B170" s="49" t="s">
         <v>283</v>
@@ -7304,7 +7385,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.95">
+    <row r="171" spans="1:3">
       <c r="A171" s="40"/>
       <c r="B171" s="49" t="s">
         <v>285</v>
@@ -7313,7 +7394,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.95">
+    <row r="172" spans="1:3">
       <c r="A172" s="40"/>
       <c r="B172" s="49" t="s">
         <v>287</v>
@@ -7322,7 +7403,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15.95">
+    <row r="173" spans="1:3">
       <c r="A173" s="40"/>
       <c r="B173" s="49" t="s">
         <v>289</v>
@@ -7331,7 +7412,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.95">
+    <row r="174" spans="1:3">
       <c r="A174" s="40"/>
       <c r="B174" s="49" t="s">
         <v>291</v>
@@ -7340,7 +7421,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="32.1">
+    <row r="175" spans="1:3" ht="29">
       <c r="A175" s="40"/>
       <c r="B175" s="49" t="s">
         <v>293</v>
@@ -7349,7 +7430,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="32.1">
+    <row r="176" spans="1:3" ht="29">
       <c r="A176" s="40"/>
       <c r="B176" s="49" t="s">
         <v>295</v>
@@ -7358,7 +7439,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.95">
+    <row r="177" spans="1:3">
       <c r="A177" s="40"/>
       <c r="B177" s="32" t="s">
         <v>271</v>
@@ -7367,7 +7448,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15.95">
+    <row r="178" spans="1:3">
       <c r="A178" s="40"/>
       <c r="B178" s="32" t="s">
         <v>147</v>
@@ -7376,7 +7457,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.95">
+    <row r="179" spans="1:3">
       <c r="A179" s="40"/>
       <c r="B179" s="32" t="s">
         <v>297</v>
@@ -7385,7 +7466,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15.95">
+    <row r="180" spans="1:3">
       <c r="A180" s="40"/>
       <c r="B180" s="49" t="s">
         <v>299</v>
@@ -7394,7 +7475,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15.95">
+    <row r="181" spans="1:3">
       <c r="A181" s="40"/>
       <c r="B181" s="49" t="s">
         <v>301</v>
@@ -7403,7 +7484,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15.95">
+    <row r="182" spans="1:3">
       <c r="A182" s="40"/>
       <c r="B182" s="32" t="s">
         <v>303</v>
@@ -7412,7 +7493,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15.95">
+    <row r="183" spans="1:3">
       <c r="A183" s="40"/>
       <c r="B183" s="32" t="s">
         <v>305</v>
@@ -7421,7 +7502,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15.95">
+    <row r="184" spans="1:3">
       <c r="A184" s="40"/>
       <c r="B184" s="32" t="s">
         <v>307</v>
@@ -7460,7 +7541,7 @@
       <c r="B191" s="38"/>
       <c r="C191" s="38"/>
     </row>
-    <row r="192" spans="1:3" ht="15.95">
+    <row r="192" spans="1:3">
       <c r="A192" s="39"/>
       <c r="B192" s="32" t="s">
         <v>311</v>
@@ -7469,7 +7550,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.95">
+    <row r="193" spans="1:3">
       <c r="A193" s="39"/>
       <c r="B193" s="32" t="s">
         <v>313</v>
@@ -7478,7 +7559,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.95">
+    <row r="194" spans="1:3">
       <c r="A194" s="39"/>
       <c r="B194" s="32" t="s">
         <v>315</v>
@@ -7487,7 +7568,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.95">
+    <row r="195" spans="1:3">
       <c r="A195" s="39"/>
       <c r="B195" s="32" t="s">
         <v>147</v>
@@ -7503,7 +7584,7 @@
       <c r="B196" s="50"/>
       <c r="C196" s="50"/>
     </row>
-    <row r="197" spans="1:3" ht="15.95">
+    <row r="197" spans="1:3">
       <c r="A197" s="40"/>
       <c r="B197" s="33" t="s">
         <v>149</v>
@@ -7519,7 +7600,7 @@
       <c r="B198" s="41"/>
       <c r="C198" s="41"/>
     </row>
-    <row r="199" spans="1:3" ht="15.95">
+    <row r="199" spans="1:3">
       <c r="A199" s="40"/>
       <c r="B199" s="32" t="s">
         <v>311</v>
@@ -7528,7 +7609,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15.95">
+    <row r="200" spans="1:3">
       <c r="A200" s="40"/>
       <c r="B200" s="32" t="s">
         <v>313</v>
@@ -7537,7 +7618,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="15.95">
+    <row r="201" spans="1:3">
       <c r="A201" s="40"/>
       <c r="B201" s="32" t="s">
         <v>315</v>
@@ -7546,7 +7627,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15.95">
+    <row r="202" spans="1:3">
       <c r="A202" s="40"/>
       <c r="B202" s="32" t="s">
         <v>147</v>
@@ -7604,14 +7685,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="86.42578125" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="24.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="86.453125" style="5" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="15.95">
+    <row r="2" spans="1:2">
       <c r="A2" s="18" t="s">
         <v>320</v>
       </c>
@@ -7634,7 +7715,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.35" customHeight="1">
+    <row r="6" spans="1:2" ht="43.4" customHeight="1">
       <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
@@ -7654,7 +7735,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.95">
+    <row r="12" spans="1:2">
       <c r="A12" s="23" t="s">
         <v>322</v>
       </c>
@@ -7672,7 +7753,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="43.35" customHeight="1">
+    <row r="15" spans="1:2" ht="43.4" customHeight="1">
       <c r="A15" s="20" t="s">
         <v>4</v>
       </c>
@@ -7687,7 +7768,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.95">
+    <row r="20" spans="1:2">
       <c r="A20" s="21" t="s">
         <v>323</v>
       </c>
@@ -7700,7 +7781,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.35" customHeight="1">
+    <row r="22" spans="1:2" ht="43.4" customHeight="1">
       <c r="A22" s="20" t="s">
         <v>4</v>
       </c>
@@ -7755,47 +7836,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F41" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F63" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="L54" sqref="L54"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" style="2" customWidth="1"/>
     <col min="4" max="4" width="28" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.81640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="19.54296875" style="2" customWidth="1"/>
     <col min="10" max="10" width="50" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="97.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="19.81640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.81640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="97.54296875" style="2" customWidth="1"/>
     <col min="16" max="16" width="34" style="2" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="77.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.42578125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="31.42578125" style="2" customWidth="1"/>
-    <col min="25" max="26" width="31.85546875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="26.42578125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="2"/>
-    <col min="29" max="29" width="77.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="17" width="25.453125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="77.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.453125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.453125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="17.453125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="31.453125" style="2" customWidth="1"/>
+    <col min="25" max="26" width="31.81640625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="26.453125" style="2" customWidth="1"/>
+    <col min="28" max="28" width="9.1796875" style="2"/>
+    <col min="29" max="29" width="77.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="56" customFormat="1" ht="48">
+    <row r="1" spans="1:29" s="56" customFormat="1" ht="44">
       <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
@@ -7876,7 +7957,7 @@
       </c>
       <c r="AC1" s="84"/>
     </row>
-    <row r="2" spans="1:29" ht="33.75">
+    <row r="2" spans="1:29" ht="43">
       <c r="B2" s="86" t="s">
         <v>344</v>
       </c>
@@ -7915,7 +7996,7 @@
       <c r="U2" s="2"/>
       <c r="AC2" s="84"/>
     </row>
-    <row r="3" spans="1:29" s="92" customFormat="1" ht="168">
+    <row r="3" spans="1:29" s="92" customFormat="1" ht="141">
       <c r="B3" s="92" t="s">
         <v>354</v>
       </c>
@@ -7952,7 +8033,7 @@
       <c r="R3" s="84"/>
       <c r="AC3" s="84"/>
     </row>
-    <row r="4" spans="1:29" s="92" customFormat="1" ht="16.5">
+    <row r="4" spans="1:29" s="92" customFormat="1" ht="16">
       <c r="A4" s="111"/>
       <c r="B4" s="111" t="s">
         <v>359</v>
@@ -7991,7 +8072,7 @@
       </c>
       <c r="AC4" s="84"/>
     </row>
-    <row r="5" spans="1:29" ht="15.95">
+    <row r="5" spans="1:29" ht="16">
       <c r="A5" s="104"/>
       <c r="B5" s="109" t="s">
         <v>362</v>
@@ -8028,7 +8109,7 @@
       </c>
       <c r="AC5" s="84"/>
     </row>
-    <row r="6" spans="1:29" ht="15.95">
+    <row r="6" spans="1:29" ht="16">
       <c r="A6" s="104"/>
       <c r="B6" s="109" t="s">
         <v>363</v>
@@ -8065,7 +8146,7 @@
       </c>
       <c r="AC6" s="84"/>
     </row>
-    <row r="7" spans="1:29" ht="91.5">
+    <row r="7" spans="1:29" ht="87.5">
       <c r="B7" s="89" t="s">
         <v>364</v>
       </c>
@@ -8103,7 +8184,7 @@
       <c r="U7" s="2"/>
       <c r="AC7" s="84"/>
     </row>
-    <row r="8" spans="1:29" ht="30.75">
+    <row r="8" spans="1:29" ht="29.5">
       <c r="B8" t="s">
         <v>369</v>
       </c>
@@ -8141,7 +8222,7 @@
       <c r="U8" s="2"/>
       <c r="AC8" s="84"/>
     </row>
-    <row r="9" spans="1:29" ht="30.75">
+    <row r="9" spans="1:29" ht="29.5">
       <c r="B9" t="s">
         <v>377</v>
       </c>
@@ -8179,7 +8260,7 @@
       <c r="U9" s="2"/>
       <c r="AC9" s="84"/>
     </row>
-    <row r="10" spans="1:29" ht="30.75">
+    <row r="10" spans="1:29" ht="44">
       <c r="B10" t="s">
         <v>385</v>
       </c>
@@ -8217,7 +8298,7 @@
       <c r="U10" s="2"/>
       <c r="AC10" s="84"/>
     </row>
-    <row r="11" spans="1:29" ht="45.75">
+    <row r="11" spans="1:29" ht="44">
       <c r="B11" s="91"/>
       <c r="I11" s="2" t="s">
         <v>387</v>
@@ -8247,7 +8328,7 @@
       <c r="U11" s="2"/>
       <c r="AC11" s="84"/>
     </row>
-    <row r="12" spans="1:29" ht="76.5">
+    <row r="12" spans="1:29" ht="58.5">
       <c r="B12" t="s">
         <v>395</v>
       </c>
@@ -8285,7 +8366,7 @@
       <c r="U12" s="2"/>
       <c r="AC12" s="84"/>
     </row>
-    <row r="13" spans="1:29" ht="76.5">
+    <row r="13" spans="1:29" ht="73">
       <c r="B13" t="s">
         <v>404</v>
       </c>
@@ -8323,7 +8404,7 @@
       <c r="U13" s="2"/>
       <c r="AC13" s="88"/>
     </row>
-    <row r="14" spans="1:29" ht="33.75">
+    <row r="14" spans="1:29" ht="43">
       <c r="B14" t="s">
         <v>409</v>
       </c>
@@ -8360,7 +8441,7 @@
       <c r="Z14" s="87"/>
       <c r="AC14" s="88"/>
     </row>
-    <row r="15" spans="1:29" ht="45.75">
+    <row r="15" spans="1:29" ht="44">
       <c r="B15" t="s">
         <v>413</v>
       </c>
@@ -8398,7 +8479,7 @@
       <c r="U15" s="2"/>
       <c r="AC15" s="84"/>
     </row>
-    <row r="16" spans="1:29" ht="167.25">
+    <row r="16" spans="1:29" ht="160">
       <c r="B16" t="s">
         <v>420</v>
       </c>
@@ -8436,7 +8517,7 @@
       <c r="U16" s="2"/>
       <c r="AC16" s="84"/>
     </row>
-    <row r="17" spans="1:29" ht="183">
+    <row r="17" spans="1:29" ht="174.5">
       <c r="B17" t="s">
         <v>425</v>
       </c>
@@ -8474,7 +8555,7 @@
       <c r="U17" s="2"/>
       <c r="AC17" s="84"/>
     </row>
-    <row r="18" spans="1:29" ht="33.75">
+    <row r="18" spans="1:29" ht="43">
       <c r="B18" t="s">
         <v>429</v>
       </c>
@@ -8511,7 +8592,7 @@
       <c r="Z18" s="87"/>
       <c r="AC18" s="84"/>
     </row>
-    <row r="19" spans="1:29" ht="15.75">
+    <row r="19" spans="1:29" ht="16">
       <c r="A19" s="104"/>
       <c r="B19" s="105" t="s">
         <v>433</v>
@@ -8548,7 +8629,7 @@
       </c>
       <c r="AC19" s="84"/>
     </row>
-    <row r="20" spans="1:29" ht="15.75">
+    <row r="20" spans="1:29" ht="16">
       <c r="A20" s="104"/>
       <c r="B20" s="105" t="s">
         <v>434</v>
@@ -8585,7 +8666,7 @@
       </c>
       <c r="AC20" s="84"/>
     </row>
-    <row r="21" spans="1:29" ht="15.75">
+    <row r="21" spans="1:29" ht="16">
       <c r="A21" s="104"/>
       <c r="B21" s="105" t="s">
         <v>435</v>
@@ -8622,7 +8703,7 @@
       </c>
       <c r="AC21" s="84"/>
     </row>
-    <row r="22" spans="1:29" ht="45.75">
+    <row r="22" spans="1:29" ht="44">
       <c r="B22" t="s">
         <v>436</v>
       </c>
@@ -8661,7 +8742,7 @@
       <c r="U22" s="2"/>
       <c r="AC22" s="84"/>
     </row>
-    <row r="23" spans="1:29" ht="45.75">
+    <row r="23" spans="1:29" ht="44">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -8700,7 +8781,7 @@
       <c r="U23" s="2"/>
       <c r="AC23" s="84"/>
     </row>
-    <row r="24" spans="1:29" ht="91.5">
+    <row r="24" spans="1:29" ht="87.5">
       <c r="B24" t="s">
         <v>447</v>
       </c>
@@ -8739,7 +8820,7 @@
       <c r="U24" s="2"/>
       <c r="AC24" s="84"/>
     </row>
-    <row r="25" spans="1:29" ht="15.75">
+    <row r="25" spans="1:29" ht="16">
       <c r="A25" s="104"/>
       <c r="B25" s="105" t="s">
         <v>455</v>
@@ -8776,7 +8857,7 @@
       </c>
       <c r="AC25" s="84"/>
     </row>
-    <row r="26" spans="1:29" ht="15.75">
+    <row r="26" spans="1:29" ht="16">
       <c r="A26" s="104"/>
       <c r="B26" s="105" t="s">
         <v>457</v>
@@ -8813,7 +8894,7 @@
       </c>
       <c r="AC26" s="84"/>
     </row>
-    <row r="27" spans="1:29" ht="15.75">
+    <row r="27" spans="1:29" ht="16">
       <c r="A27" s="104"/>
       <c r="B27" s="105" t="s">
         <v>458</v>
@@ -8850,7 +8931,7 @@
       </c>
       <c r="AC27" s="84"/>
     </row>
-    <row r="28" spans="1:29" ht="15.75">
+    <row r="28" spans="1:29" ht="16">
       <c r="A28" s="104"/>
       <c r="B28" s="105" t="s">
         <v>459</v>
@@ -8887,7 +8968,7 @@
       </c>
       <c r="AC28" s="84"/>
     </row>
-    <row r="29" spans="1:29" ht="15.75">
+    <row r="29" spans="1:29" ht="16">
       <c r="A29" s="104"/>
       <c r="B29" s="105" t="s">
         <v>460</v>
@@ -8924,7 +9005,7 @@
       </c>
       <c r="AC29" s="84"/>
     </row>
-    <row r="30" spans="1:29" ht="15.75">
+    <row r="30" spans="1:29" ht="16">
       <c r="A30" s="104"/>
       <c r="B30" s="105" t="s">
         <v>461</v>
@@ -8961,7 +9042,7 @@
       </c>
       <c r="AC30" s="84"/>
     </row>
-    <row r="31" spans="1:29" ht="15.75">
+    <row r="31" spans="1:29" ht="16">
       <c r="A31" s="104"/>
       <c r="B31" s="105" t="s">
         <v>462</v>
@@ -8998,7 +9079,7 @@
       </c>
       <c r="AC31" s="84"/>
     </row>
-    <row r="32" spans="1:29" ht="15.75">
+    <row r="32" spans="1:29" ht="16">
       <c r="A32" s="104"/>
       <c r="B32" s="105" t="s">
         <v>463</v>
@@ -9035,7 +9116,7 @@
       </c>
       <c r="AC32" s="84"/>
     </row>
-    <row r="33" spans="1:29" ht="15.75">
+    <row r="33" spans="1:29" ht="16">
       <c r="A33" s="104"/>
       <c r="B33" s="105" t="s">
         <v>464</v>
@@ -9072,7 +9153,7 @@
       </c>
       <c r="AC33" s="84"/>
     </row>
-    <row r="34" spans="1:29" ht="15.75">
+    <row r="34" spans="1:29" ht="16">
       <c r="A34" s="104"/>
       <c r="B34" s="105" t="s">
         <v>465</v>
@@ -9109,7 +9190,7 @@
       </c>
       <c r="AC34" s="84"/>
     </row>
-    <row r="35" spans="1:29" ht="15.75">
+    <row r="35" spans="1:29" ht="16">
       <c r="B35" t="s">
         <v>466</v>
       </c>
@@ -9146,7 +9227,7 @@
       <c r="U35" s="2"/>
       <c r="AC35" s="84"/>
     </row>
-    <row r="36" spans="1:29" ht="15.75">
+    <row r="36" spans="1:29" ht="16">
       <c r="B36" t="s">
         <v>474</v>
       </c>
@@ -9183,7 +9264,7 @@
       <c r="U36" s="2"/>
       <c r="AC36" s="84"/>
     </row>
-    <row r="37" spans="1:29" ht="15.75">
+    <row r="37" spans="1:29" ht="16">
       <c r="A37" s="104"/>
       <c r="B37" s="105" t="s">
         <v>480</v>
@@ -9220,7 +9301,7 @@
       </c>
       <c r="AC37" s="84"/>
     </row>
-    <row r="38" spans="1:29" ht="15.75">
+    <row r="38" spans="1:29" ht="16">
       <c r="A38" s="104"/>
       <c r="B38" s="105" t="s">
         <v>100</v>
@@ -9257,7 +9338,7 @@
       </c>
       <c r="AC38" s="84"/>
     </row>
-    <row r="39" spans="1:29" ht="15.75">
+    <row r="39" spans="1:29" ht="16">
       <c r="A39" s="104"/>
       <c r="B39" s="105" t="s">
         <v>481</v>
@@ -9294,7 +9375,7 @@
       </c>
       <c r="AC39" s="84"/>
     </row>
-    <row r="40" spans="1:29" ht="15.75">
+    <row r="40" spans="1:29" ht="16">
       <c r="A40" s="104"/>
       <c r="B40" s="105" t="s">
         <v>482</v>
@@ -9331,7 +9412,7 @@
       </c>
       <c r="AC40" s="84"/>
     </row>
-    <row r="41" spans="1:29" ht="15.75">
+    <row r="41" spans="1:29" ht="16">
       <c r="A41" s="104"/>
       <c r="B41" s="105" t="s">
         <v>483</v>
@@ -9368,7 +9449,7 @@
       </c>
       <c r="AC41" s="84"/>
     </row>
-    <row r="42" spans="1:29" ht="15.75">
+    <row r="42" spans="1:29" ht="16">
       <c r="A42" s="104"/>
       <c r="B42" s="105" t="s">
         <v>354</v>
@@ -9405,7 +9486,7 @@
       </c>
       <c r="AC42" s="84"/>
     </row>
-    <row r="43" spans="1:29" ht="15.75">
+    <row r="43" spans="1:29" ht="16">
       <c r="A43" s="104"/>
       <c r="B43" s="105" t="s">
         <v>484</v>
@@ -9442,7 +9523,7 @@
       </c>
       <c r="AC43" s="84"/>
     </row>
-    <row r="44" spans="1:29" ht="15.75">
+    <row r="44" spans="1:29" ht="16">
       <c r="A44" s="104"/>
       <c r="B44" s="105" t="s">
         <v>485</v>
@@ -9479,7 +9560,7 @@
       </c>
       <c r="AC44" s="84"/>
     </row>
-    <row r="45" spans="1:29" ht="15.75">
+    <row r="45" spans="1:29" ht="16">
       <c r="A45" s="104"/>
       <c r="B45" s="105" t="s">
         <v>487</v>
@@ -9516,7 +9597,7 @@
       </c>
       <c r="AC45" s="84"/>
     </row>
-    <row r="46" spans="1:29" ht="15.75">
+    <row r="46" spans="1:29" ht="16">
       <c r="A46" s="104"/>
       <c r="B46" s="105" t="s">
         <v>488</v>
@@ -9551,7 +9632,7 @@
       </c>
       <c r="AC46" s="84"/>
     </row>
-    <row r="47" spans="1:29" ht="15.75">
+    <row r="47" spans="1:29" ht="16">
       <c r="A47" s="104"/>
       <c r="B47" s="105" t="s">
         <v>489</v>
@@ -9588,7 +9669,7 @@
       </c>
       <c r="AC47" s="84"/>
     </row>
-    <row r="48" spans="1:29" ht="15.75">
+    <row r="48" spans="1:29" ht="16">
       <c r="A48" s="104"/>
       <c r="B48" s="105" t="s">
         <v>490</v>
@@ -9625,7 +9706,7 @@
       </c>
       <c r="AC48" s="84"/>
     </row>
-    <row r="49" spans="1:29" ht="15.75">
+    <row r="49" spans="1:29" ht="16">
       <c r="A49" s="104"/>
       <c r="B49" s="105" t="s">
         <v>491</v>
@@ -9662,7 +9743,7 @@
       </c>
       <c r="AC49" s="84"/>
     </row>
-    <row r="50" spans="1:29" ht="15.75">
+    <row r="50" spans="1:29" ht="16">
       <c r="A50" s="104"/>
       <c r="B50" s="105" t="s">
         <v>492</v>
@@ -9699,7 +9780,7 @@
       </c>
       <c r="AC50" s="84"/>
     </row>
-    <row r="51" spans="1:29" ht="15.75">
+    <row r="51" spans="1:29" ht="16">
       <c r="A51" s="104"/>
       <c r="B51" s="105" t="s">
         <v>493</v>
@@ -9736,7 +9817,7 @@
       </c>
       <c r="AC51" s="88"/>
     </row>
-    <row r="52" spans="1:29" ht="30.75">
+    <row r="52" spans="1:29" ht="29.5">
       <c r="B52" t="s">
         <v>495</v>
       </c>
@@ -9774,7 +9855,7 @@
       <c r="U52" s="2"/>
       <c r="AC52" s="84"/>
     </row>
-    <row r="53" spans="1:29" ht="45.75">
+    <row r="53" spans="1:29" ht="44">
       <c r="B53" t="s">
         <v>501</v>
       </c>
@@ -9813,7 +9894,7 @@
       <c r="U53" s="2"/>
       <c r="AC53" s="84"/>
     </row>
-    <row r="54" spans="1:29" ht="91.5">
+    <row r="54" spans="1:29" ht="87.5">
       <c r="B54" s="86" t="s">
         <v>505</v>
       </c>
@@ -9841,19 +9922,19 @@
       <c r="P54" s="100" t="s">
         <v>510</v>
       </c>
-      <c r="Q54" s="123" t="s">
+      <c r="Q54" s="117" t="s">
         <v>511</v>
       </c>
       <c r="R54" s="84"/>
       <c r="U54" s="2"/>
       <c r="AC54" s="84"/>
     </row>
-    <row r="55" spans="1:29" ht="60.75">
+    <row r="55" spans="1:29" ht="58.5">
       <c r="B55" s="89"/>
       <c r="I55" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J55" s="124" t="s">
+      <c r="J55" s="118" t="s">
         <v>512</v>
       </c>
       <c r="K55" s="103" t="s">
@@ -9878,12 +9959,12 @@
       <c r="U55" s="2"/>
       <c r="AC55" s="84"/>
     </row>
-    <row r="56" spans="1:29" ht="45.75">
+    <row r="56" spans="1:29" ht="44">
       <c r="B56" s="89"/>
       <c r="I56" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J56" s="124" t="s">
+      <c r="J56" s="118" t="s">
         <v>517</v>
       </c>
       <c r="K56" s="103" t="s">
@@ -9908,12 +9989,12 @@
       <c r="U56" s="2"/>
       <c r="AC56" s="84"/>
     </row>
-    <row r="57" spans="1:29" ht="30.75">
+    <row r="57" spans="1:29" ht="29.5">
       <c r="B57" s="89"/>
       <c r="I57" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J57" s="124" t="s">
+      <c r="J57" s="118" t="s">
         <v>521</v>
       </c>
       <c r="K57" s="103" t="s">
@@ -9938,12 +10019,12 @@
       <c r="U57" s="2"/>
       <c r="AC57" s="84"/>
     </row>
-    <row r="58" spans="1:29" ht="30.75">
+    <row r="58" spans="1:29" ht="29.5">
       <c r="B58" s="89"/>
       <c r="I58" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J58" s="124" t="s">
+      <c r="J58" s="118" t="s">
         <v>527</v>
       </c>
       <c r="K58" s="103" t="s">
@@ -9955,7 +10036,7 @@
       <c r="M58" s="100" t="s">
         <v>350</v>
       </c>
-      <c r="O58" s="125" t="s">
+      <c r="O58" s="119" t="s">
         <v>529</v>
       </c>
       <c r="P58" s="2" t="s">
@@ -9968,12 +10049,12 @@
       <c r="U58" s="2"/>
       <c r="AC58" s="84"/>
     </row>
-    <row r="59" spans="1:29" ht="45.75">
+    <row r="59" spans="1:29" ht="44">
       <c r="B59" s="89"/>
       <c r="I59" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J59" s="124" t="s">
+      <c r="J59" s="118" t="s">
         <v>530</v>
       </c>
       <c r="K59" s="103" t="s">
@@ -9998,12 +10079,12 @@
       <c r="U59" s="2"/>
       <c r="AC59" s="84"/>
     </row>
-    <row r="60" spans="1:29" ht="167.25">
+    <row r="60" spans="1:29" ht="160">
       <c r="B60" s="89"/>
       <c r="I60" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J60" s="124" t="s">
+      <c r="J60" s="118" t="s">
         <v>533</v>
       </c>
       <c r="K60" s="103" t="s">
@@ -10028,12 +10109,12 @@
       <c r="U60" s="2"/>
       <c r="AC60" s="84"/>
     </row>
-    <row r="61" spans="1:29" ht="137.25">
+    <row r="61" spans="1:29" ht="116.5">
       <c r="B61" s="89"/>
       <c r="I61" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J61" s="124" t="s">
+      <c r="J61" s="118" t="s">
         <v>538</v>
       </c>
       <c r="K61" s="103" t="s">
@@ -10058,12 +10139,12 @@
       <c r="U61" s="2"/>
       <c r="AC61" s="84"/>
     </row>
-    <row r="62" spans="1:29" ht="91.5">
+    <row r="62" spans="1:29" ht="87.5">
       <c r="B62" s="89"/>
       <c r="I62" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J62" s="124" t="s">
+      <c r="J62" s="118" t="s">
         <v>542</v>
       </c>
       <c r="K62" s="103" t="s">
@@ -10088,12 +10169,12 @@
       <c r="U62" s="2"/>
       <c r="AC62" s="84"/>
     </row>
-    <row r="63" spans="1:29" ht="91.5">
+    <row r="63" spans="1:29" ht="73">
       <c r="B63" s="89"/>
       <c r="I63" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="J63" s="124" t="s">
+      <c r="J63" s="118" t="s">
         <v>547</v>
       </c>
       <c r="K63" s="103" t="s">
@@ -10118,7 +10199,7 @@
       <c r="U63" s="2"/>
       <c r="AC63" s="84"/>
     </row>
-    <row r="64" spans="1:29" ht="15.75">
+    <row r="64" spans="1:29" ht="16">
       <c r="B64" s="89"/>
       <c r="I64" s="86"/>
       <c r="J64" s="86"/>
@@ -10132,7 +10213,7 @@
       <c r="U64" s="2"/>
       <c r="AC64" s="84"/>
     </row>
-    <row r="65" spans="2:29" ht="15.75">
+    <row r="65" spans="2:29" ht="16">
       <c r="B65" s="89"/>
       <c r="I65" s="86"/>
       <c r="J65" s="86"/>
@@ -10146,7 +10227,7 @@
       <c r="U65" s="2"/>
       <c r="AC65" s="84"/>
     </row>
-    <row r="66" spans="2:29" ht="15.75">
+    <row r="66" spans="2:29" ht="16">
       <c r="B66" s="89"/>
       <c r="I66" s="86"/>
       <c r="J66" s="86"/>
@@ -10160,7 +10241,7 @@
       <c r="U66" s="2"/>
       <c r="AC66" s="84"/>
     </row>
-    <row r="67" spans="2:29" ht="15.75">
+    <row r="67" spans="2:29" ht="16">
       <c r="B67" s="89"/>
       <c r="I67" s="86"/>
       <c r="J67" s="86"/>
@@ -10173,7 +10254,7 @@
       <c r="U67" s="2"/>
       <c r="AC67" s="84"/>
     </row>
-    <row r="68" spans="2:29" ht="15.75">
+    <row r="68" spans="2:29" ht="16">
       <c r="B68" s="89"/>
       <c r="I68" s="86"/>
       <c r="J68" s="86"/>
@@ -10186,7 +10267,7 @@
       <c r="U68" s="2"/>
       <c r="AC68" s="84"/>
     </row>
-    <row r="69" spans="2:29" ht="15.75">
+    <row r="69" spans="2:29" ht="16">
       <c r="B69" s="89"/>
       <c r="I69" s="86"/>
       <c r="J69" s="86"/>
@@ -10199,7 +10280,7 @@
       <c r="U69" s="2"/>
       <c r="AC69" s="84"/>
     </row>
-    <row r="70" spans="2:29" ht="15.75">
+    <row r="70" spans="2:29" ht="16">
       <c r="B70" s="89"/>
       <c r="I70" s="86"/>
       <c r="J70" s="86"/>
@@ -10209,7 +10290,7 @@
       <c r="U70" s="2"/>
       <c r="AC70" s="84"/>
     </row>
-    <row r="71" spans="2:29" ht="15.75">
+    <row r="71" spans="2:29" ht="16">
       <c r="B71" s="89"/>
       <c r="I71" s="86"/>
       <c r="J71" s="86"/>
@@ -10223,7 +10304,7 @@
       <c r="U71" s="2"/>
       <c r="AC71" s="84"/>
     </row>
-    <row r="72" spans="2:29" ht="15.75">
+    <row r="72" spans="2:29" ht="16">
       <c r="B72" s="89"/>
       <c r="I72" s="86"/>
       <c r="J72" s="86"/>
@@ -10237,7 +10318,7 @@
       <c r="U72" s="2"/>
       <c r="AC72" s="84"/>
     </row>
-    <row r="73" spans="2:29" ht="15.75">
+    <row r="73" spans="2:29" ht="16">
       <c r="B73" s="89"/>
       <c r="I73" s="86"/>
       <c r="J73" s="86"/>
@@ -10251,7 +10332,7 @@
       <c r="U73" s="2"/>
       <c r="AC73" s="84"/>
     </row>
-    <row r="74" spans="2:29" ht="15.75">
+    <row r="74" spans="2:29" ht="16">
       <c r="B74" s="89"/>
       <c r="I74" s="86"/>
       <c r="J74" s="86"/>
@@ -10264,7 +10345,7 @@
       <c r="U74" s="2"/>
       <c r="AC74" s="84"/>
     </row>
-    <row r="75" spans="2:29" ht="15.75">
+    <row r="75" spans="2:29" ht="16">
       <c r="B75" s="89"/>
       <c r="I75" s="86"/>
       <c r="J75" s="86"/>
@@ -10274,7 +10355,7 @@
       <c r="U75" s="2"/>
       <c r="AC75" s="84"/>
     </row>
-    <row r="76" spans="2:29" ht="15.75">
+    <row r="76" spans="2:29" ht="16">
       <c r="B76" s="89"/>
       <c r="I76" s="86"/>
       <c r="J76" s="86"/>
@@ -10284,7 +10365,7 @@
       <c r="U76" s="2"/>
       <c r="AC76" s="84"/>
     </row>
-    <row r="77" spans="2:29" ht="15.75">
+    <row r="77" spans="2:29" ht="16">
       <c r="B77" s="89"/>
       <c r="I77" s="86"/>
       <c r="J77" s="86"/>
@@ -10295,7 +10376,7 @@
       <c r="U77" s="2"/>
       <c r="AC77" s="84"/>
     </row>
-    <row r="78" spans="2:29" ht="15.75">
+    <row r="78" spans="2:29" ht="16">
       <c r="B78" s="89"/>
       <c r="I78" s="86"/>
       <c r="J78" s="86"/>
@@ -10309,7 +10390,7 @@
       <c r="U78" s="2"/>
       <c r="AC78" s="84"/>
     </row>
-    <row r="79" spans="2:29" ht="15.75">
+    <row r="79" spans="2:29" ht="16">
       <c r="B79" s="89"/>
       <c r="I79" s="86"/>
       <c r="J79" s="86"/>
@@ -10323,7 +10404,7 @@
       <c r="U79" s="2"/>
       <c r="AC79" s="84"/>
     </row>
-    <row r="80" spans="2:29" ht="15.75">
+    <row r="80" spans="2:29" ht="16">
       <c r="B80" s="89"/>
       <c r="I80" s="86"/>
       <c r="J80" s="86"/>
@@ -10336,7 +10417,7 @@
       <c r="U80" s="2"/>
       <c r="AC80" s="84"/>
     </row>
-    <row r="81" spans="2:29" ht="15.75">
+    <row r="81" spans="2:29" ht="16">
       <c r="B81" s="89"/>
       <c r="I81" s="86"/>
       <c r="J81" s="86"/>
@@ -10347,7 +10428,7 @@
       <c r="U81" s="2"/>
       <c r="AC81" s="84"/>
     </row>
-    <row r="82" spans="2:29" ht="15.75">
+    <row r="82" spans="2:29" ht="16">
       <c r="B82" s="89"/>
       <c r="I82" s="86"/>
       <c r="J82" s="86"/>
@@ -10360,7 +10441,7 @@
       <c r="U82" s="2"/>
       <c r="AC82" s="84"/>
     </row>
-    <row r="83" spans="2:29" ht="15.75">
+    <row r="83" spans="2:29" ht="16">
       <c r="B83" s="89"/>
       <c r="I83" s="86"/>
       <c r="J83" s="86"/>
@@ -10370,7 +10451,7 @@
       <c r="U83" s="2"/>
       <c r="AC83" s="84"/>
     </row>
-    <row r="84" spans="2:29" ht="15.75">
+    <row r="84" spans="2:29" ht="16">
       <c r="B84" s="89"/>
       <c r="I84" s="86"/>
       <c r="J84" s="86"/>
@@ -10380,7 +10461,7 @@
       <c r="U84" s="2"/>
       <c r="AC84" s="84"/>
     </row>
-    <row r="85" spans="2:29" ht="15.75">
+    <row r="85" spans="2:29" ht="16">
       <c r="B85" s="89"/>
       <c r="I85" s="86"/>
       <c r="J85" s="86"/>
@@ -10393,7 +10474,7 @@
       <c r="U85" s="2"/>
       <c r="AC85" s="84"/>
     </row>
-    <row r="86" spans="2:29" ht="15.75">
+    <row r="86" spans="2:29" ht="16">
       <c r="B86" s="89"/>
       <c r="I86" s="86"/>
       <c r="J86" s="86"/>
@@ -10404,7 +10485,7 @@
       <c r="U86" s="2"/>
       <c r="AC86" s="84"/>
     </row>
-    <row r="87" spans="2:29" ht="15.75">
+    <row r="87" spans="2:29" ht="16">
       <c r="B87" s="89"/>
       <c r="I87" s="86"/>
       <c r="J87" s="86"/>
@@ -10414,7 +10495,7 @@
       <c r="U87" s="2"/>
       <c r="AC87" s="84"/>
     </row>
-    <row r="88" spans="2:29" ht="15.75">
+    <row r="88" spans="2:29" ht="16">
       <c r="B88" s="89"/>
       <c r="I88" s="86"/>
       <c r="J88" s="86"/>
@@ -10424,7 +10505,7 @@
       <c r="U88" s="2"/>
       <c r="AC88" s="84"/>
     </row>
-    <row r="89" spans="2:29" ht="15.75">
+    <row r="89" spans="2:29" ht="16">
       <c r="B89" s="89"/>
       <c r="I89" s="86"/>
       <c r="J89" s="86"/>
@@ -10437,7 +10518,7 @@
       <c r="U89" s="2"/>
       <c r="AC89" s="84"/>
     </row>
-    <row r="90" spans="2:29" ht="15.75">
+    <row r="90" spans="2:29" ht="16">
       <c r="B90" s="91"/>
       <c r="I90" s="86"/>
       <c r="J90" s="86"/>
@@ -10450,7 +10531,7 @@
       <c r="U90" s="2"/>
       <c r="AC90" s="84"/>
     </row>
-    <row r="91" spans="2:29" ht="15.75">
+    <row r="91" spans="2:29" ht="16">
       <c r="B91" s="89"/>
       <c r="I91" s="86"/>
       <c r="J91" s="86"/>
@@ -10464,7 +10545,7 @@
       <c r="U91" s="2"/>
       <c r="AC91" s="84"/>
     </row>
-    <row r="92" spans="2:29" ht="15.75">
+    <row r="92" spans="2:29" ht="16">
       <c r="B92" s="89"/>
       <c r="I92" s="86"/>
       <c r="J92" s="86"/>
@@ -10478,7 +10559,7 @@
       <c r="U92" s="2"/>
       <c r="AC92" s="84"/>
     </row>
-    <row r="93" spans="2:29" ht="15.75">
+    <row r="93" spans="2:29" ht="16">
       <c r="B93" s="89"/>
       <c r="I93" s="86"/>
       <c r="J93" s="86"/>
@@ -10492,7 +10573,7 @@
       <c r="U93" s="2"/>
       <c r="AC93" s="84"/>
     </row>
-    <row r="94" spans="2:29" ht="15.75">
+    <row r="94" spans="2:29" ht="16">
       <c r="B94" s="89"/>
       <c r="I94" s="86"/>
       <c r="J94" s="86"/>
@@ -10506,7 +10587,7 @@
       <c r="U94" s="2"/>
       <c r="AC94" s="84"/>
     </row>
-    <row r="95" spans="2:29" ht="15.75">
+    <row r="95" spans="2:29" ht="16">
       <c r="B95" s="89"/>
       <c r="I95" s="86"/>
       <c r="J95" s="86"/>
@@ -10520,7 +10601,7 @@
       <c r="U95" s="2"/>
       <c r="AC95" s="84"/>
     </row>
-    <row r="96" spans="2:29" ht="15.75">
+    <row r="96" spans="2:29" ht="16">
       <c r="B96" s="89"/>
       <c r="I96" s="86"/>
       <c r="J96" s="86"/>
@@ -10534,7 +10615,7 @@
       <c r="U96" s="2"/>
       <c r="AC96" s="84"/>
     </row>
-    <row r="97" spans="2:29" ht="15.75">
+    <row r="97" spans="2:29" ht="16">
       <c r="B97" s="89"/>
       <c r="I97" s="86"/>
       <c r="J97" s="86"/>
@@ -10547,7 +10628,7 @@
       <c r="U97" s="2"/>
       <c r="AC97" s="84"/>
     </row>
-    <row r="98" spans="2:29" ht="15.75">
+    <row r="98" spans="2:29" ht="16">
       <c r="B98" s="89"/>
       <c r="I98" s="86"/>
       <c r="J98" s="86"/>
@@ -10560,7 +10641,7 @@
       <c r="U98" s="2"/>
       <c r="AC98" s="84"/>
     </row>
-    <row r="99" spans="2:29" ht="15.75">
+    <row r="99" spans="2:29" ht="16">
       <c r="B99" s="89"/>
       <c r="I99" s="86"/>
       <c r="J99" s="86"/>
@@ -10574,7 +10655,7 @@
       <c r="U99" s="2"/>
       <c r="AC99" s="84"/>
     </row>
-    <row r="100" spans="2:29" ht="15.75">
+    <row r="100" spans="2:29" ht="16">
       <c r="B100" s="89"/>
       <c r="I100" s="86"/>
       <c r="J100" s="86"/>
@@ -10587,7 +10668,7 @@
       <c r="U100" s="2"/>
       <c r="AC100" s="84"/>
     </row>
-    <row r="101" spans="2:29" ht="15.75">
+    <row r="101" spans="2:29" ht="16">
       <c r="B101" s="89"/>
       <c r="I101" s="86"/>
       <c r="J101" s="86"/>
@@ -10600,7 +10681,7 @@
       <c r="U101" s="2"/>
       <c r="AC101" s="84"/>
     </row>
-    <row r="102" spans="2:29" ht="15.75">
+    <row r="102" spans="2:29" ht="16">
       <c r="B102" s="89"/>
       <c r="I102" s="86"/>
       <c r="J102" s="86"/>
@@ -10610,7 +10691,7 @@
       <c r="U102" s="2"/>
       <c r="AC102" s="84"/>
     </row>
-    <row r="103" spans="2:29" ht="15.75">
+    <row r="103" spans="2:29" ht="16">
       <c r="B103" s="89"/>
       <c r="I103" s="86"/>
       <c r="J103" s="86"/>
@@ -10620,7 +10701,7 @@
       <c r="U103" s="2"/>
       <c r="AC103" s="84"/>
     </row>
-    <row r="104" spans="2:29" ht="15.75">
+    <row r="104" spans="2:29" ht="16">
       <c r="B104" s="89"/>
       <c r="I104" s="86"/>
       <c r="J104" s="86"/>
@@ -10632,7 +10713,7 @@
       <c r="U104" s="2"/>
       <c r="AC104" s="84"/>
     </row>
-    <row r="105" spans="2:29" ht="15.75">
+    <row r="105" spans="2:29" ht="16">
       <c r="B105" s="89"/>
       <c r="I105" s="86"/>
       <c r="J105" s="86"/>
@@ -10643,7 +10724,7 @@
       <c r="U105" s="2"/>
       <c r="AC105" s="84"/>
     </row>
-    <row r="106" spans="2:29" ht="15.75">
+    <row r="106" spans="2:29" ht="16">
       <c r="B106" s="89"/>
       <c r="I106" s="86"/>
       <c r="J106" s="86"/>
@@ -10653,7 +10734,7 @@
       <c r="U106" s="2"/>
       <c r="AC106" s="84"/>
     </row>
-    <row r="107" spans="2:29" ht="15.75">
+    <row r="107" spans="2:29" ht="16">
       <c r="B107" s="89"/>
       <c r="I107" s="86"/>
       <c r="J107" s="86"/>
@@ -10666,7 +10747,7 @@
       <c r="U107" s="2"/>
       <c r="AC107" s="84"/>
     </row>
-    <row r="108" spans="2:29" ht="15.75">
+    <row r="108" spans="2:29" ht="16">
       <c r="B108" s="89"/>
       <c r="I108" s="86"/>
       <c r="J108" s="86"/>
@@ -10679,7 +10760,7 @@
       <c r="U108" s="2"/>
       <c r="AC108" s="84"/>
     </row>
-    <row r="109" spans="2:29" ht="15.75">
+    <row r="109" spans="2:29" ht="16">
       <c r="B109" s="89"/>
       <c r="I109" s="86"/>
       <c r="J109" s="86"/>
@@ -10692,7 +10773,7 @@
       <c r="U109" s="2"/>
       <c r="AC109" s="84"/>
     </row>
-    <row r="110" spans="2:29" ht="15.75">
+    <row r="110" spans="2:29" ht="16">
       <c r="B110" s="89"/>
       <c r="I110" s="86"/>
       <c r="J110" s="86"/>
@@ -10705,7 +10786,7 @@
       <c r="U110" s="2"/>
       <c r="AC110" s="84"/>
     </row>
-    <row r="111" spans="2:29" ht="15.75">
+    <row r="111" spans="2:29" ht="16">
       <c r="B111" s="89"/>
       <c r="I111" s="86"/>
       <c r="J111" s="86"/>
@@ -10715,7 +10796,7 @@
       <c r="U111" s="2"/>
       <c r="AC111" s="84"/>
     </row>
-    <row r="112" spans="2:29" ht="15.75">
+    <row r="112" spans="2:29" ht="16">
       <c r="B112" s="89"/>
       <c r="I112" s="86"/>
       <c r="J112" s="86"/>
@@ -10726,7 +10807,7 @@
       <c r="U112" s="2"/>
       <c r="AC112" s="84"/>
     </row>
-    <row r="113" spans="2:29" ht="15.75">
+    <row r="113" spans="2:29" ht="16">
       <c r="B113" s="89"/>
       <c r="I113" s="86"/>
       <c r="J113" s="86"/>
@@ -10738,7 +10819,7 @@
       <c r="U113" s="2"/>
       <c r="AC113" s="84"/>
     </row>
-    <row r="114" spans="2:29" ht="15.75">
+    <row r="114" spans="2:29" ht="16">
       <c r="B114" s="89"/>
       <c r="I114" s="86"/>
       <c r="J114" s="86"/>
@@ -10750,7 +10831,7 @@
       <c r="U114" s="2"/>
       <c r="AC114" s="84"/>
     </row>
-    <row r="115" spans="2:29" ht="15.75">
+    <row r="115" spans="2:29" ht="16">
       <c r="B115" s="89"/>
       <c r="I115" s="86"/>
       <c r="J115" s="86"/>
@@ -10763,7 +10844,7 @@
       <c r="U115" s="2"/>
       <c r="AC115" s="84"/>
     </row>
-    <row r="116" spans="2:29" ht="15.75">
+    <row r="116" spans="2:29" ht="16">
       <c r="B116" s="89"/>
       <c r="I116" s="86"/>
       <c r="J116" s="86"/>
@@ -10776,7 +10857,7 @@
       <c r="U116" s="2"/>
       <c r="AC116" s="84"/>
     </row>
-    <row r="117" spans="2:29" ht="15.75">
+    <row r="117" spans="2:29" ht="16">
       <c r="B117" s="89"/>
       <c r="I117" s="86"/>
       <c r="J117" s="86"/>
@@ -10789,7 +10870,7 @@
       <c r="U117" s="2"/>
       <c r="AC117" s="84"/>
     </row>
-    <row r="118" spans="2:29" ht="15.75">
+    <row r="118" spans="2:29" ht="16">
       <c r="B118" s="89"/>
       <c r="I118" s="86"/>
       <c r="J118" s="86"/>
@@ -10802,7 +10883,7 @@
       <c r="U118" s="2"/>
       <c r="AC118" s="84"/>
     </row>
-    <row r="119" spans="2:29" ht="15.75">
+    <row r="119" spans="2:29" ht="16">
       <c r="B119" s="89"/>
       <c r="I119" s="86"/>
       <c r="J119" s="86"/>
@@ -10815,7 +10896,7 @@
       <c r="U119" s="2"/>
       <c r="AC119" s="84"/>
     </row>
-    <row r="120" spans="2:29" ht="15.75">
+    <row r="120" spans="2:29" ht="16">
       <c r="B120" s="89"/>
       <c r="I120" s="86"/>
       <c r="J120" s="86"/>
@@ -10828,7 +10909,7 @@
       <c r="U120" s="2"/>
       <c r="AC120" s="84"/>
     </row>
-    <row r="121" spans="2:29" ht="15.75">
+    <row r="121" spans="2:29" ht="16">
       <c r="B121" s="89"/>
       <c r="I121" s="86"/>
       <c r="J121" s="86"/>
@@ -10841,7 +10922,7 @@
       <c r="U121" s="2"/>
       <c r="AC121" s="84"/>
     </row>
-    <row r="122" spans="2:29" ht="15.75">
+    <row r="122" spans="2:29" ht="16">
       <c r="B122" s="89"/>
       <c r="I122" s="86"/>
       <c r="J122" s="86"/>
@@ -10854,7 +10935,7 @@
       <c r="U122" s="2"/>
       <c r="AC122" s="84"/>
     </row>
-    <row r="123" spans="2:29" ht="15.75">
+    <row r="123" spans="2:29" ht="16">
       <c r="B123" s="89"/>
       <c r="I123" s="86"/>
       <c r="J123" s="86"/>
@@ -10867,7 +10948,7 @@
       <c r="U123" s="2"/>
       <c r="AC123" s="84"/>
     </row>
-    <row r="124" spans="2:29" ht="15.75">
+    <row r="124" spans="2:29" ht="16">
       <c r="B124" s="89"/>
       <c r="I124" s="86"/>
       <c r="J124" s="86"/>
@@ -10881,7 +10962,7 @@
       <c r="U124" s="2"/>
       <c r="AC124" s="84"/>
     </row>
-    <row r="125" spans="2:29" ht="15.75">
+    <row r="125" spans="2:29" ht="16">
       <c r="B125" s="89"/>
       <c r="I125" s="86"/>
       <c r="J125" s="86"/>
@@ -10895,7 +10976,7 @@
       <c r="U125" s="2"/>
       <c r="AC125" s="84"/>
     </row>
-    <row r="126" spans="2:29" ht="15.75">
+    <row r="126" spans="2:29" ht="16">
       <c r="B126" s="89"/>
       <c r="I126" s="86"/>
       <c r="J126" s="86"/>
@@ -10909,7 +10990,7 @@
       <c r="U126" s="2"/>
       <c r="AC126" s="84"/>
     </row>
-    <row r="127" spans="2:29" ht="15.75">
+    <row r="127" spans="2:29" ht="16">
       <c r="B127" s="89"/>
       <c r="I127" s="86"/>
       <c r="J127" s="86"/>
@@ -10922,7 +11003,7 @@
       <c r="U127" s="2"/>
       <c r="AC127" s="84"/>
     </row>
-    <row r="128" spans="2:29" ht="15.75">
+    <row r="128" spans="2:29" ht="16">
       <c r="B128" s="89"/>
       <c r="I128" s="86"/>
       <c r="J128" s="89"/>
@@ -10935,7 +11016,7 @@
       <c r="U128" s="2"/>
       <c r="AC128" s="84"/>
     </row>
-    <row r="129" spans="2:29" ht="15.75">
+    <row r="129" spans="2:29" ht="16">
       <c r="B129" s="89"/>
       <c r="I129" s="86"/>
       <c r="J129" s="86"/>
@@ -10945,7 +11026,7 @@
       <c r="U129" s="2"/>
       <c r="AC129" s="84"/>
     </row>
-    <row r="130" spans="2:29" ht="15.75">
+    <row r="130" spans="2:29" ht="16">
       <c r="B130" s="89"/>
       <c r="I130" s="86"/>
       <c r="J130" s="86"/>
@@ -10958,7 +11039,7 @@
       <c r="U130" s="2"/>
       <c r="AC130" s="84"/>
     </row>
-    <row r="131" spans="2:29" ht="15.75">
+    <row r="131" spans="2:29" ht="16">
       <c r="B131" s="89"/>
       <c r="I131" s="86"/>
       <c r="J131" s="86"/>
@@ -10971,7 +11052,7 @@
       <c r="U131" s="2"/>
       <c r="AC131" s="84"/>
     </row>
-    <row r="132" spans="2:29" ht="15.75">
+    <row r="132" spans="2:29" ht="16">
       <c r="B132" s="89"/>
       <c r="I132" s="86"/>
       <c r="J132" s="86"/>
@@ -10985,7 +11066,7 @@
       <c r="U132" s="2"/>
       <c r="AC132" s="84"/>
     </row>
-    <row r="133" spans="2:29" ht="15.75">
+    <row r="133" spans="2:29" ht="16">
       <c r="B133" s="89"/>
       <c r="I133" s="86"/>
       <c r="J133" s="86"/>
@@ -10999,7 +11080,7 @@
       <c r="U133" s="2"/>
       <c r="AC133" s="84"/>
     </row>
-    <row r="134" spans="2:29" ht="15.75">
+    <row r="134" spans="2:29" ht="16">
       <c r="B134" s="89"/>
       <c r="I134" s="86"/>
       <c r="J134" s="86"/>
@@ -11013,7 +11094,7 @@
       <c r="U134" s="2"/>
       <c r="AC134" s="84"/>
     </row>
-    <row r="135" spans="2:29" ht="15.75">
+    <row r="135" spans="2:29" ht="16">
       <c r="B135" s="89"/>
       <c r="I135" s="86"/>
       <c r="J135" s="86"/>
@@ -11027,7 +11108,7 @@
       <c r="U135" s="2"/>
       <c r="AC135" s="84"/>
     </row>
-    <row r="136" spans="2:29" ht="15.75">
+    <row r="136" spans="2:29" ht="16">
       <c r="B136" s="89"/>
       <c r="I136" s="86"/>
       <c r="J136" s="86"/>
@@ -11041,7 +11122,7 @@
       <c r="U136" s="2"/>
       <c r="AC136" s="85"/>
     </row>
-    <row r="137" spans="2:29" ht="15.75">
+    <row r="137" spans="2:29" ht="16">
       <c r="B137" s="89"/>
       <c r="I137" s="86"/>
       <c r="J137" s="86"/>
@@ -11055,7 +11136,7 @@
       <c r="U137" s="2"/>
       <c r="AC137" s="84"/>
     </row>
-    <row r="138" spans="2:29" ht="15.75">
+    <row r="138" spans="2:29" ht="16">
       <c r="B138" s="89"/>
       <c r="I138" s="86"/>
       <c r="J138" s="86"/>
@@ -11069,7 +11150,7 @@
       <c r="U138" s="2"/>
       <c r="AC138" s="88"/>
     </row>
-    <row r="139" spans="2:29" ht="15.75">
+    <row r="139" spans="2:29" ht="16">
       <c r="B139" s="89"/>
       <c r="I139" s="86"/>
       <c r="J139" s="86"/>
@@ -11083,7 +11164,7 @@
       <c r="U139" s="2"/>
       <c r="AC139" s="84"/>
     </row>
-    <row r="140" spans="2:29" ht="15.75">
+    <row r="140" spans="2:29" ht="16">
       <c r="B140" s="89"/>
       <c r="I140" s="86"/>
       <c r="J140" s="86"/>
@@ -11097,7 +11178,7 @@
       <c r="U140" s="2"/>
       <c r="AC140" s="84"/>
     </row>
-    <row r="141" spans="2:29" ht="15.75">
+    <row r="141" spans="2:29" ht="16">
       <c r="B141" s="89"/>
       <c r="I141" s="86"/>
       <c r="J141" s="86"/>
@@ -11111,7 +11192,7 @@
       <c r="U141" s="2"/>
       <c r="AC141" s="84"/>
     </row>
-    <row r="142" spans="2:29" ht="15.75">
+    <row r="142" spans="2:29" ht="16">
       <c r="B142" s="89"/>
       <c r="I142" s="86"/>
       <c r="J142" s="86"/>
@@ -11125,7 +11206,7 @@
       <c r="U142" s="2"/>
       <c r="AC142" s="84"/>
     </row>
-    <row r="143" spans="2:29" ht="15.75">
+    <row r="143" spans="2:29" ht="16">
       <c r="B143" s="89"/>
       <c r="I143" s="86"/>
       <c r="J143" s="86"/>
@@ -11139,7 +11220,7 @@
       <c r="U143" s="2"/>
       <c r="AC143" s="84"/>
     </row>
-    <row r="144" spans="2:29" ht="15.75">
+    <row r="144" spans="2:29" ht="16">
       <c r="B144" s="89"/>
       <c r="I144" s="86"/>
       <c r="J144" s="86"/>
@@ -11153,7 +11234,7 @@
       <c r="U144" s="2"/>
       <c r="AC144" s="84"/>
     </row>
-    <row r="145" spans="2:29" ht="15.75">
+    <row r="145" spans="2:29" ht="16">
       <c r="B145" s="89"/>
       <c r="I145" s="86"/>
       <c r="J145" s="86"/>
@@ -11167,7 +11248,7 @@
       <c r="U145" s="2"/>
       <c r="AC145" s="84"/>
     </row>
-    <row r="146" spans="2:29" ht="15.75">
+    <row r="146" spans="2:29" ht="16">
       <c r="B146" s="89"/>
       <c r="I146" s="86"/>
       <c r="J146" s="86"/>
@@ -11181,7 +11262,7 @@
       <c r="U146" s="2"/>
       <c r="AC146" s="84"/>
     </row>
-    <row r="147" spans="2:29" ht="15.75">
+    <row r="147" spans="2:29" ht="16">
       <c r="B147" s="89"/>
       <c r="I147" s="86"/>
       <c r="J147" s="86"/>
@@ -11195,7 +11276,7 @@
       <c r="U147" s="2"/>
       <c r="AC147" s="84"/>
     </row>
-    <row r="148" spans="2:29" ht="15.75">
+    <row r="148" spans="2:29" ht="16">
       <c r="B148" s="89"/>
       <c r="I148" s="86"/>
       <c r="J148" s="86"/>
@@ -11209,7 +11290,7 @@
       <c r="U148" s="2"/>
       <c r="AC148" s="84"/>
     </row>
-    <row r="149" spans="2:29" ht="15.75">
+    <row r="149" spans="2:29" ht="16">
       <c r="B149" s="89"/>
       <c r="I149" s="86"/>
       <c r="J149" s="86"/>
@@ -11223,7 +11304,7 @@
       <c r="U149" s="2"/>
       <c r="AC149" s="84"/>
     </row>
-    <row r="150" spans="2:29" ht="15.75">
+    <row r="150" spans="2:29" ht="16">
       <c r="B150" s="89"/>
       <c r="I150" s="86"/>
       <c r="J150" s="86"/>
@@ -11237,7 +11318,7 @@
       <c r="U150" s="2"/>
       <c r="AC150" s="84"/>
     </row>
-    <row r="151" spans="2:29" ht="15.75">
+    <row r="151" spans="2:29" ht="16">
       <c r="B151" s="89"/>
       <c r="I151" s="86"/>
       <c r="J151" s="86"/>
@@ -11251,7 +11332,7 @@
       <c r="U151" s="2"/>
       <c r="AC151" s="84"/>
     </row>
-    <row r="152" spans="2:29" ht="15.75">
+    <row r="152" spans="2:29" ht="16">
       <c r="B152" s="89"/>
       <c r="I152" s="86"/>
       <c r="J152" s="86"/>
@@ -11265,7 +11346,7 @@
       <c r="U152" s="2"/>
       <c r="AC152" s="84"/>
     </row>
-    <row r="153" spans="2:29" ht="15.75">
+    <row r="153" spans="2:29" ht="16">
       <c r="B153" s="89"/>
       <c r="I153" s="86"/>
       <c r="J153" s="86"/>
@@ -11279,7 +11360,7 @@
       <c r="U153" s="2"/>
       <c r="AC153" s="84"/>
     </row>
-    <row r="154" spans="2:29" ht="15.75">
+    <row r="154" spans="2:29" ht="16">
       <c r="B154" s="89"/>
       <c r="I154" s="86"/>
       <c r="J154" s="86"/>
@@ -11293,7 +11374,7 @@
       <c r="U154" s="2"/>
       <c r="AC154" s="84"/>
     </row>
-    <row r="155" spans="2:29" ht="15.75">
+    <row r="155" spans="2:29" ht="16">
       <c r="B155" s="89"/>
       <c r="I155" s="86"/>
       <c r="J155" s="86"/>
@@ -11307,7 +11388,7 @@
       <c r="U155" s="2"/>
       <c r="AC155" s="84"/>
     </row>
-    <row r="156" spans="2:29" ht="15.75">
+    <row r="156" spans="2:29" ht="16">
       <c r="B156" s="89"/>
       <c r="I156" s="86"/>
       <c r="J156" s="86"/>
@@ -11321,7 +11402,7 @@
       <c r="U156" s="2"/>
       <c r="AC156" s="84"/>
     </row>
-    <row r="157" spans="2:29" ht="15.75">
+    <row r="157" spans="2:29" ht="16">
       <c r="B157" s="89"/>
       <c r="I157" s="86"/>
       <c r="J157" s="86"/>
@@ -11335,7 +11416,7 @@
       <c r="U157" s="2"/>
       <c r="AC157" s="84"/>
     </row>
-    <row r="158" spans="2:29" ht="15.75">
+    <row r="158" spans="2:29" ht="16">
       <c r="B158" s="89"/>
       <c r="I158" s="86"/>
       <c r="J158" s="86"/>
@@ -11349,7 +11430,7 @@
       <c r="U158" s="2"/>
       <c r="AC158" s="84"/>
     </row>
-    <row r="159" spans="2:29" ht="15.75">
+    <row r="159" spans="2:29" ht="16">
       <c r="B159" s="89"/>
       <c r="I159" s="86"/>
       <c r="J159" s="86"/>
@@ -11363,7 +11444,7 @@
       <c r="U159" s="2"/>
       <c r="AC159" s="84"/>
     </row>
-    <row r="160" spans="2:29" ht="15.75">
+    <row r="160" spans="2:29" ht="16">
       <c r="B160" s="89"/>
       <c r="I160" s="86"/>
       <c r="J160" s="86"/>
@@ -11374,7 +11455,7 @@
       <c r="U160" s="2"/>
       <c r="AC160" s="84"/>
     </row>
-    <row r="161" spans="2:29" ht="15.75">
+    <row r="161" spans="2:29" ht="16">
       <c r="B161" s="89"/>
       <c r="I161" s="86"/>
       <c r="J161" s="90"/>
@@ -11385,7 +11466,7 @@
       <c r="U161" s="2"/>
       <c r="AC161" s="84"/>
     </row>
-    <row r="162" spans="2:29" ht="15.75">
+    <row r="162" spans="2:29" ht="16">
       <c r="B162" s="89"/>
       <c r="I162" s="86"/>
       <c r="J162" s="90"/>
@@ -11396,7 +11477,7 @@
       <c r="U162" s="2"/>
       <c r="AC162" s="84"/>
     </row>
-    <row r="163" spans="2:29" ht="15.75">
+    <row r="163" spans="2:29" ht="16">
       <c r="B163" s="89"/>
       <c r="I163" s="86"/>
       <c r="J163" s="86"/>
@@ -11407,7 +11488,7 @@
       <c r="U163" s="2"/>
       <c r="AC163" s="84"/>
     </row>
-    <row r="164" spans="2:29" ht="15.75">
+    <row r="164" spans="2:29" ht="16">
       <c r="B164" s="89"/>
       <c r="I164" s="86"/>
       <c r="J164" s="86"/>
@@ -11418,7 +11499,7 @@
       <c r="U164" s="2"/>
       <c r="AC164" s="84"/>
     </row>
-    <row r="165" spans="2:29" ht="15.75">
+    <row r="165" spans="2:29" ht="16">
       <c r="B165" s="89"/>
       <c r="I165" s="86"/>
       <c r="J165" s="86"/>
@@ -11429,7 +11510,7 @@
       <c r="U165" s="2"/>
       <c r="AC165" s="84"/>
     </row>
-    <row r="166" spans="2:29" ht="15.75">
+    <row r="166" spans="2:29" ht="16">
       <c r="B166" s="89"/>
       <c r="I166" s="86"/>
       <c r="J166" s="86"/>
@@ -11443,7 +11524,7 @@
       <c r="U166" s="2"/>
       <c r="AC166" s="84"/>
     </row>
-    <row r="167" spans="2:29" ht="15.75">
+    <row r="167" spans="2:29" ht="16">
       <c r="B167" s="89"/>
       <c r="D167" s="86"/>
       <c r="I167" s="86"/>
@@ -11458,7 +11539,7 @@
       <c r="U167" s="2"/>
       <c r="AC167" s="84"/>
     </row>
-    <row r="168" spans="2:29" ht="15.75">
+    <row r="168" spans="2:29" ht="16">
       <c r="B168" s="89"/>
       <c r="D168" s="86"/>
       <c r="I168" s="86"/>
@@ -11473,7 +11554,7 @@
       <c r="U168" s="2"/>
       <c r="AC168" s="84"/>
     </row>
-    <row r="169" spans="2:29" ht="15.75">
+    <row r="169" spans="2:29" ht="16">
       <c r="B169" s="89"/>
       <c r="D169" s="86"/>
       <c r="I169" s="86"/>
@@ -11488,7 +11569,7 @@
       <c r="U169" s="2"/>
       <c r="AC169" s="84"/>
     </row>
-    <row r="170" spans="2:29" ht="15.75">
+    <row r="170" spans="2:29" ht="16">
       <c r="B170" s="89"/>
       <c r="D170" s="86"/>
       <c r="I170" s="86"/>
@@ -11503,7 +11584,7 @@
       <c r="U170" s="2"/>
       <c r="AC170" s="84"/>
     </row>
-    <row r="171" spans="2:29" ht="15.75">
+    <row r="171" spans="2:29" ht="16">
       <c r="B171" s="89"/>
       <c r="D171" s="86"/>
       <c r="I171" s="86"/>
@@ -11518,7 +11599,7 @@
       <c r="U171" s="2"/>
       <c r="AC171" s="84"/>
     </row>
-    <row r="172" spans="2:29" ht="15.75">
+    <row r="172" spans="2:29" ht="16">
       <c r="B172" s="89"/>
       <c r="D172" s="86"/>
       <c r="I172" s="86"/>
@@ -11533,7 +11614,7 @@
       <c r="U172" s="2"/>
       <c r="AC172" s="84"/>
     </row>
-    <row r="173" spans="2:29" ht="15.75">
+    <row r="173" spans="2:29" ht="16">
       <c r="B173" s="89"/>
       <c r="D173" s="86"/>
       <c r="I173" s="86"/>
@@ -11548,7 +11629,7 @@
       <c r="U173" s="2"/>
       <c r="AC173" s="84"/>
     </row>
-    <row r="174" spans="2:29" ht="15.75">
+    <row r="174" spans="2:29" ht="16">
       <c r="B174" s="86"/>
       <c r="C174" s="86"/>
       <c r="D174" s="86"/>
@@ -11565,7 +11646,7 @@
       <c r="U174" s="2"/>
       <c r="AC174" s="84"/>
     </row>
-    <row r="175" spans="2:29" ht="15.75">
+    <row r="175" spans="2:29" ht="16">
       <c r="B175" s="91"/>
       <c r="I175" s="86"/>
       <c r="J175" s="86"/>
@@ -11579,7 +11660,7 @@
       <c r="U175" s="2"/>
       <c r="AC175" s="84"/>
     </row>
-    <row r="176" spans="2:29" ht="15.75">
+    <row r="176" spans="2:29" ht="16">
       <c r="B176" s="89"/>
       <c r="I176" s="86"/>
       <c r="J176" s="86"/>
@@ -11593,7 +11674,7 @@
       <c r="U176" s="2"/>
       <c r="AC176" s="84"/>
     </row>
-    <row r="177" spans="2:29" ht="15.75">
+    <row r="177" spans="2:29" ht="16">
       <c r="B177" s="89"/>
       <c r="I177" s="86"/>
       <c r="J177" s="86"/>
@@ -11607,7 +11688,7 @@
       <c r="U177" s="2"/>
       <c r="AC177" s="84"/>
     </row>
-    <row r="178" spans="2:29" ht="15.75">
+    <row r="178" spans="2:29" ht="16">
       <c r="B178" s="89"/>
       <c r="I178" s="86"/>
       <c r="J178" s="86"/>
@@ -11621,7 +11702,7 @@
       <c r="U178" s="2"/>
       <c r="AC178" s="84"/>
     </row>
-    <row r="179" spans="2:29" ht="15.75">
+    <row r="179" spans="2:29" ht="16">
       <c r="B179" s="89"/>
       <c r="I179" s="86"/>
       <c r="J179" s="86"/>
@@ -11635,7 +11716,7 @@
       <c r="U179" s="2"/>
       <c r="AC179" s="84"/>
     </row>
-    <row r="180" spans="2:29" ht="15.75">
+    <row r="180" spans="2:29" ht="16">
       <c r="B180" s="89"/>
       <c r="I180" s="86"/>
       <c r="J180" s="86"/>
@@ -11649,7 +11730,7 @@
       <c r="U180" s="2"/>
       <c r="AC180" s="84"/>
     </row>
-    <row r="181" spans="2:29" ht="15.75">
+    <row r="181" spans="2:29" ht="16">
       <c r="B181" s="91"/>
       <c r="I181" s="86"/>
       <c r="J181" s="86"/>
@@ -11663,7 +11744,7 @@
       <c r="U181" s="2"/>
       <c r="AC181" s="84"/>
     </row>
-    <row r="182" spans="2:29" ht="15.75">
+    <row r="182" spans="2:29" ht="16">
       <c r="B182" s="89"/>
       <c r="I182" s="86"/>
       <c r="J182" s="86"/>
@@ -11677,7 +11758,7 @@
       <c r="U182" s="2"/>
       <c r="AC182" s="84"/>
     </row>
-    <row r="183" spans="2:29" ht="15.75">
+    <row r="183" spans="2:29" ht="16">
       <c r="B183" s="89"/>
       <c r="I183" s="86"/>
       <c r="J183" s="86"/>
@@ -11690,7 +11771,7 @@
       <c r="U183" s="2"/>
       <c r="AC183" s="84"/>
     </row>
-    <row r="184" spans="2:29" ht="15.75">
+    <row r="184" spans="2:29" ht="16">
       <c r="B184" s="89"/>
       <c r="I184" s="86"/>
       <c r="J184" s="86"/>
@@ -11704,7 +11785,7 @@
       <c r="U184" s="2"/>
       <c r="AC184" s="84"/>
     </row>
-    <row r="185" spans="2:29" ht="15.75">
+    <row r="185" spans="2:29" ht="16">
       <c r="B185" s="89"/>
       <c r="I185" s="86"/>
       <c r="J185" s="86"/>
@@ -11718,7 +11799,7 @@
       <c r="U185" s="2"/>
       <c r="AC185" s="84"/>
     </row>
-    <row r="186" spans="2:29" ht="15.75">
+    <row r="186" spans="2:29" ht="16">
       <c r="B186" s="89"/>
       <c r="I186" s="86"/>
       <c r="J186" s="86"/>
@@ -11732,7 +11813,7 @@
       <c r="U186" s="2"/>
       <c r="AC186" s="84"/>
     </row>
-    <row r="187" spans="2:29" ht="15.75">
+    <row r="187" spans="2:29" ht="16">
       <c r="B187" s="89"/>
       <c r="I187" s="86"/>
       <c r="J187" s="86"/>
@@ -11746,7 +11827,7 @@
       <c r="U187" s="2"/>
       <c r="AC187" s="84"/>
     </row>
-    <row r="188" spans="2:29" ht="15.75">
+    <row r="188" spans="2:29" ht="16">
       <c r="B188" s="89"/>
       <c r="I188" s="86"/>
       <c r="J188" s="86"/>
@@ -11759,7 +11840,7 @@
       <c r="U188" s="2"/>
       <c r="AC188" s="84"/>
     </row>
-    <row r="189" spans="2:29" ht="15.75">
+    <row r="189" spans="2:29" ht="16">
       <c r="B189" s="89"/>
       <c r="I189" s="86"/>
       <c r="J189" s="86"/>
@@ -11773,7 +11854,7 @@
       <c r="U189" s="2"/>
       <c r="AC189" s="84"/>
     </row>
-    <row r="190" spans="2:29" ht="15.75">
+    <row r="190" spans="2:29" ht="16">
       <c r="B190" s="89"/>
       <c r="I190" s="86"/>
       <c r="J190" s="86"/>
@@ -11787,7 +11868,7 @@
       <c r="U190" s="2"/>
       <c r="AC190" s="84"/>
     </row>
-    <row r="191" spans="2:29" ht="15.75">
+    <row r="191" spans="2:29" ht="16">
       <c r="B191" s="89"/>
       <c r="I191" s="86"/>
       <c r="J191" s="86"/>
@@ -11801,7 +11882,7 @@
       <c r="U191" s="2"/>
       <c r="AC191" s="84"/>
     </row>
-    <row r="192" spans="2:29" ht="15.75">
+    <row r="192" spans="2:29" ht="16">
       <c r="B192" s="89"/>
       <c r="I192" s="86"/>
       <c r="J192" s="86"/>
@@ -11814,7 +11895,7 @@
       <c r="U192" s="2"/>
       <c r="AC192" s="84"/>
     </row>
-    <row r="193" spans="2:29" ht="15.75">
+    <row r="193" spans="2:29" ht="16">
       <c r="B193" s="89"/>
       <c r="I193" s="86"/>
       <c r="J193" s="86"/>
@@ -11828,7 +11909,7 @@
       <c r="U193" s="2"/>
       <c r="AC193" s="84"/>
     </row>
-    <row r="194" spans="2:29" ht="15.75">
+    <row r="194" spans="2:29" ht="16">
       <c r="B194" s="89"/>
       <c r="I194" s="86"/>
       <c r="J194" s="86"/>
@@ -11842,7 +11923,7 @@
       <c r="U194" s="2"/>
       <c r="AC194" s="84"/>
     </row>
-    <row r="195" spans="2:29" ht="15.75">
+    <row r="195" spans="2:29" ht="16">
       <c r="B195" s="89"/>
       <c r="I195" s="86"/>
       <c r="J195" s="86"/>
@@ -11855,7 +11936,7 @@
       <c r="U195" s="2"/>
       <c r="AC195" s="84"/>
     </row>
-    <row r="196" spans="2:29" ht="15.75">
+    <row r="196" spans="2:29" ht="16">
       <c r="B196" s="91"/>
       <c r="I196" s="86"/>
       <c r="J196" s="86"/>
@@ -11868,7 +11949,7 @@
       <c r="U196" s="2"/>
       <c r="AC196" s="84"/>
     </row>
-    <row r="197" spans="2:29" ht="15.75">
+    <row r="197" spans="2:29" ht="16">
       <c r="B197" s="89"/>
       <c r="I197" s="86"/>
       <c r="J197" s="86"/>
@@ -11882,7 +11963,7 @@
       <c r="U197" s="2"/>
       <c r="AC197" s="88"/>
     </row>
-    <row r="198" spans="2:29" ht="15.75">
+    <row r="198" spans="2:29" ht="16">
       <c r="B198" s="89"/>
       <c r="I198" s="86"/>
       <c r="J198" s="86"/>
@@ -11895,7 +11976,7 @@
       <c r="U198" s="2"/>
       <c r="AC198" s="84"/>
     </row>
-    <row r="199" spans="2:29" ht="15.75">
+    <row r="199" spans="2:29" ht="16">
       <c r="B199" s="89"/>
       <c r="I199" s="86"/>
       <c r="J199" s="86"/>
@@ -11908,7 +11989,7 @@
       <c r="U199" s="2"/>
       <c r="AC199" s="88"/>
     </row>
-    <row r="200" spans="2:29" ht="15.75">
+    <row r="200" spans="2:29" ht="16">
       <c r="B200" s="89"/>
       <c r="I200" s="86"/>
       <c r="J200" s="86"/>
@@ -11921,7 +12002,7 @@
       <c r="U200" s="2"/>
       <c r="AC200" s="84"/>
     </row>
-    <row r="201" spans="2:29" ht="15.75">
+    <row r="201" spans="2:29" ht="16">
       <c r="B201" s="89"/>
       <c r="I201" s="86"/>
       <c r="J201" s="86"/>
@@ -11935,7 +12016,7 @@
       <c r="U201" s="2"/>
       <c r="AC201" s="84"/>
     </row>
-    <row r="202" spans="2:29" ht="15.75">
+    <row r="202" spans="2:29" ht="16">
       <c r="B202" s="89"/>
       <c r="I202" s="86"/>
       <c r="J202" s="86"/>
@@ -11948,7 +12029,7 @@
       <c r="U202" s="2"/>
       <c r="AC202" s="84"/>
     </row>
-    <row r="203" spans="2:29" ht="15.75">
+    <row r="203" spans="2:29" ht="16">
       <c r="B203" s="89"/>
       <c r="I203" s="86"/>
       <c r="J203" s="86"/>
@@ -11962,7 +12043,7 @@
       <c r="U203" s="2"/>
       <c r="AC203" s="84"/>
     </row>
-    <row r="204" spans="2:29" ht="15.75">
+    <row r="204" spans="2:29" ht="16">
       <c r="B204" s="89"/>
       <c r="I204" s="86"/>
       <c r="J204" s="86"/>
@@ -11976,7 +12057,7 @@
       <c r="U204" s="2"/>
       <c r="AC204" s="84"/>
     </row>
-    <row r="205" spans="2:29" ht="15.75">
+    <row r="205" spans="2:29" ht="16">
       <c r="B205" s="89"/>
       <c r="I205" s="86"/>
       <c r="J205" s="86"/>
@@ -11990,7 +12071,7 @@
       <c r="U205" s="2"/>
       <c r="AC205" s="84"/>
     </row>
-    <row r="206" spans="2:29" ht="15.75">
+    <row r="206" spans="2:29" ht="16">
       <c r="B206" s="89"/>
       <c r="I206" s="86"/>
       <c r="J206" s="86"/>
@@ -12003,7 +12084,7 @@
       <c r="U206" s="2"/>
       <c r="AC206" s="84"/>
     </row>
-    <row r="207" spans="2:29" ht="15.75">
+    <row r="207" spans="2:29" ht="16">
       <c r="B207" s="89"/>
       <c r="E207" s="81"/>
       <c r="I207" s="86"/>
@@ -12018,7 +12099,7 @@
       <c r="U207" s="2"/>
       <c r="AC207" s="84"/>
     </row>
-    <row r="208" spans="2:29" ht="15.75">
+    <row r="208" spans="2:29" ht="16">
       <c r="B208" s="89"/>
       <c r="I208" s="86"/>
       <c r="J208" s="86"/>
@@ -12032,7 +12113,7 @@
       <c r="U208" s="2"/>
       <c r="AC208" s="84"/>
     </row>
-    <row r="209" spans="2:29" ht="15.75">
+    <row r="209" spans="2:29" ht="16">
       <c r="B209" s="89"/>
       <c r="I209" s="86"/>
       <c r="J209" s="86"/>
@@ -12046,7 +12127,7 @@
       <c r="U209" s="2"/>
       <c r="AC209" s="84"/>
     </row>
-    <row r="210" spans="2:29" ht="15.75">
+    <row r="210" spans="2:29" ht="16">
       <c r="B210" s="89"/>
       <c r="I210" s="86"/>
       <c r="J210" s="86"/>
@@ -12060,7 +12141,7 @@
       <c r="U210" s="2"/>
       <c r="AC210" s="84"/>
     </row>
-    <row r="211" spans="2:29" ht="15.75">
+    <row r="211" spans="2:29" ht="16">
       <c r="B211" s="89"/>
       <c r="I211" s="86"/>
       <c r="J211" s="86"/>
@@ -12074,7 +12155,7 @@
       <c r="U211" s="2"/>
       <c r="AC211" s="84"/>
     </row>
-    <row r="212" spans="2:29" ht="15.75">
+    <row r="212" spans="2:29" ht="16">
       <c r="B212" s="89"/>
       <c r="I212" s="86"/>
       <c r="J212" s="86"/>
@@ -12088,7 +12169,7 @@
       <c r="U212" s="2"/>
       <c r="AC212" s="84"/>
     </row>
-    <row r="213" spans="2:29" ht="15.75">
+    <row r="213" spans="2:29" ht="16">
       <c r="B213" s="86"/>
       <c r="C213" s="86"/>
       <c r="D213" s="86"/>
@@ -12103,7 +12184,7 @@
       <c r="U213" s="2"/>
       <c r="AC213" s="84"/>
     </row>
-    <row r="214" spans="2:29" ht="15.75">
+    <row r="214" spans="2:29" ht="16">
       <c r="B214" s="86"/>
       <c r="C214" s="86"/>
       <c r="D214" s="86"/>
@@ -12116,7 +12197,7 @@
       <c r="U214" s="2"/>
       <c r="AC214" s="84"/>
     </row>
-    <row r="215" spans="2:29" ht="15.75">
+    <row r="215" spans="2:29" ht="16">
       <c r="B215" s="86"/>
       <c r="C215" s="86"/>
       <c r="D215" s="86"/>
@@ -12133,7 +12214,7 @@
       <c r="U215" s="2"/>
       <c r="AC215" s="84"/>
     </row>
-    <row r="216" spans="2:29" ht="15.75">
+    <row r="216" spans="2:29" ht="16">
       <c r="B216" s="86"/>
       <c r="C216" s="86"/>
       <c r="D216" s="86"/>
@@ -12150,7 +12231,7 @@
       <c r="U216" s="2"/>
       <c r="AC216" s="84"/>
     </row>
-    <row r="217" spans="2:29" ht="15.75">
+    <row r="217" spans="2:29" ht="16">
       <c r="B217" s="86"/>
       <c r="C217" s="86"/>
       <c r="D217" s="86"/>
@@ -12164,7 +12245,7 @@
       <c r="U217" s="2"/>
       <c r="AC217" s="84"/>
     </row>
-    <row r="218" spans="2:29" ht="15.75">
+    <row r="218" spans="2:29" ht="16">
       <c r="B218" s="86"/>
       <c r="C218" s="86"/>
       <c r="D218" s="86"/>
@@ -12181,7 +12262,7 @@
       <c r="U218" s="2"/>
       <c r="AC218" s="84"/>
     </row>
-    <row r="219" spans="2:29" ht="15.75">
+    <row r="219" spans="2:29" ht="16">
       <c r="B219" s="86"/>
       <c r="C219" s="86"/>
       <c r="D219" s="86"/>
@@ -12198,7 +12279,7 @@
       <c r="U219" s="2"/>
       <c r="AC219" s="84"/>
     </row>
-    <row r="220" spans="2:29" ht="15.75">
+    <row r="220" spans="2:29" ht="16">
       <c r="B220" s="86"/>
       <c r="C220" s="86"/>
       <c r="D220" s="86"/>
@@ -12215,7 +12296,7 @@
       <c r="U220" s="2"/>
       <c r="AC220" s="84"/>
     </row>
-    <row r="221" spans="2:29" ht="15.75">
+    <row r="221" spans="2:29" ht="16">
       <c r="B221" s="89"/>
       <c r="I221" s="86"/>
       <c r="J221" s="86"/>
@@ -12229,7 +12310,7 @@
       <c r="U221" s="2"/>
       <c r="AC221" s="84"/>
     </row>
-    <row r="222" spans="2:29" ht="15.75">
+    <row r="222" spans="2:29" ht="16">
       <c r="I222" s="86"/>
       <c r="J222" s="86"/>
       <c r="K222" s="86"/>
@@ -12242,7 +12323,7 @@
       <c r="U222" s="2"/>
       <c r="AC222" s="84"/>
     </row>
-    <row r="223" spans="2:29" ht="15.75">
+    <row r="223" spans="2:29" ht="16">
       <c r="B223" s="101"/>
       <c r="I223" s="86"/>
       <c r="J223" s="86"/>
@@ -12256,7 +12337,7 @@
       <c r="U223" s="2"/>
       <c r="AC223" s="84"/>
     </row>
-    <row r="224" spans="2:29" ht="15.75">
+    <row r="224" spans="2:29" ht="16">
       <c r="B224" s="89"/>
       <c r="I224" s="86"/>
       <c r="J224" s="86"/>
@@ -12268,7 +12349,7 @@
       <c r="U224" s="2"/>
       <c r="AC224" s="84"/>
     </row>
-    <row r="225" spans="2:29" ht="15.75">
+    <row r="225" spans="2:29" ht="16">
       <c r="B225" s="89"/>
       <c r="I225" s="86"/>
       <c r="J225" s="86"/>
@@ -12282,7 +12363,7 @@
       <c r="U225" s="2"/>
       <c r="AC225" s="88"/>
     </row>
-    <row r="226" spans="2:29" ht="15.75">
+    <row r="226" spans="2:29" ht="16">
       <c r="B226" s="89"/>
       <c r="I226" s="86"/>
       <c r="J226" s="86"/>
@@ -12296,7 +12377,7 @@
       <c r="U226" s="2"/>
       <c r="AC226" s="84"/>
     </row>
-    <row r="227" spans="2:29" ht="15.75">
+    <row r="227" spans="2:29" ht="16">
       <c r="B227" s="89"/>
       <c r="I227" s="86"/>
       <c r="J227" s="86"/>
@@ -12310,7 +12391,7 @@
       <c r="U227" s="2"/>
       <c r="AC227" s="84"/>
     </row>
-    <row r="228" spans="2:29" ht="15.75">
+    <row r="228" spans="2:29" ht="16">
       <c r="B228" s="89"/>
       <c r="I228" s="86"/>
       <c r="J228" s="86"/>
@@ -12324,7 +12405,7 @@
       <c r="U228" s="2"/>
       <c r="AC228" s="84"/>
     </row>
-    <row r="229" spans="2:29" ht="15.75">
+    <row r="229" spans="2:29" ht="16">
       <c r="B229" s="89"/>
       <c r="J229" s="86"/>
       <c r="K229" s="86"/>
@@ -12336,7 +12417,7 @@
       <c r="U229" s="2"/>
       <c r="AC229" s="84"/>
     </row>
-    <row r="230" spans="2:29" ht="15.75">
+    <row r="230" spans="2:29" ht="16">
       <c r="B230" s="89"/>
       <c r="J230" s="86"/>
       <c r="K230" s="86"/>
@@ -12348,7 +12429,7 @@
       <c r="U230" s="2"/>
       <c r="AC230" s="84"/>
     </row>
-    <row r="231" spans="2:29" ht="15.75">
+    <row r="231" spans="2:29" ht="16">
       <c r="B231" s="89"/>
       <c r="J231" s="86"/>
       <c r="K231" s="86"/>
@@ -12359,7 +12440,7 @@
       <c r="U231" s="2"/>
       <c r="AC231" s="84"/>
     </row>
-    <row r="232" spans="2:29" ht="15.75">
+    <row r="232" spans="2:29" ht="16">
       <c r="B232" s="89"/>
       <c r="J232" s="86"/>
       <c r="K232" s="86"/>
@@ -12367,7 +12448,7 @@
       <c r="U232" s="2"/>
       <c r="AC232" s="84"/>
     </row>
-    <row r="233" spans="2:29" ht="15.75">
+    <row r="233" spans="2:29" ht="16">
       <c r="B233" s="89"/>
       <c r="J233" s="86"/>
       <c r="K233" s="86"/>
@@ -12379,7 +12460,7 @@
       <c r="U233" s="2"/>
       <c r="AC233" s="84"/>
     </row>
-    <row r="234" spans="2:29" ht="15.75">
+    <row r="234" spans="2:29" ht="16">
       <c r="B234" s="102"/>
       <c r="C234" s="103"/>
       <c r="D234" s="85"/>
@@ -12389,7 +12470,7 @@
       <c r="U234" s="2"/>
       <c r="AC234" s="84"/>
     </row>
-    <row r="235" spans="2:29" ht="15.75">
+    <row r="235" spans="2:29" ht="16">
       <c r="B235" s="102"/>
       <c r="C235" s="103"/>
       <c r="D235" s="85"/>
@@ -12399,7 +12480,7 @@
       <c r="U235" s="2"/>
       <c r="AC235" s="84"/>
     </row>
-    <row r="236" spans="2:29" ht="15.75">
+    <row r="236" spans="2:29" ht="16">
       <c r="B236" s="102"/>
       <c r="C236" s="103"/>
       <c r="D236" s="85"/>
@@ -12409,7 +12490,7 @@
       <c r="U236" s="2"/>
       <c r="AC236" s="84"/>
     </row>
-    <row r="237" spans="2:29" ht="15.75">
+    <row r="237" spans="2:29" ht="16">
       <c r="B237" s="102"/>
       <c r="C237" s="103"/>
       <c r="D237" s="85"/>
@@ -12419,7 +12500,7 @@
       <c r="U237" s="2"/>
       <c r="AC237" s="84"/>
     </row>
-    <row r="238" spans="2:29" ht="15.75">
+    <row r="238" spans="2:29" ht="16">
       <c r="B238" s="102"/>
       <c r="C238" s="103"/>
       <c r="D238" s="85"/>
@@ -12429,7 +12510,7 @@
       <c r="U238" s="2"/>
       <c r="AC238" s="84"/>
     </row>
-    <row r="239" spans="2:29" ht="15.75">
+    <row r="239" spans="2:29" ht="16">
       <c r="B239" s="102"/>
       <c r="C239" s="103"/>
       <c r="D239" s="85"/>
@@ -12439,7 +12520,7 @@
       <c r="U239" s="2"/>
       <c r="AC239" s="84"/>
     </row>
-    <row r="240" spans="2:29" ht="15.75">
+    <row r="240" spans="2:29" ht="16">
       <c r="B240" s="102"/>
       <c r="C240" s="103"/>
       <c r="D240" s="85"/>
@@ -12449,7 +12530,7 @@
       <c r="U240" s="2"/>
       <c r="AC240" s="84"/>
     </row>
-    <row r="241" spans="2:29" ht="15.75">
+    <row r="241" spans="2:29" ht="16">
       <c r="B241" s="102"/>
       <c r="C241" s="103"/>
       <c r="D241" s="85"/>
@@ -12459,7 +12540,7 @@
       <c r="U241" s="2"/>
       <c r="AC241" s="84"/>
     </row>
-    <row r="242" spans="2:29" ht="15.75">
+    <row r="242" spans="2:29" ht="16">
       <c r="B242" s="102"/>
       <c r="C242" s="103"/>
       <c r="D242" s="85"/>
@@ -12469,7 +12550,7 @@
       <c r="U242" s="2"/>
       <c r="AC242" s="84"/>
     </row>
-    <row r="243" spans="2:29" ht="15.75">
+    <row r="243" spans="2:29" ht="16">
       <c r="B243" s="102"/>
       <c r="C243" s="103"/>
       <c r="D243" s="85"/>
@@ -12479,7 +12560,7 @@
       <c r="U243" s="2"/>
       <c r="AC243" s="84"/>
     </row>
-    <row r="244" spans="2:29" ht="15.75">
+    <row r="244" spans="2:29" ht="16">
       <c r="B244" s="102"/>
       <c r="C244" s="103"/>
       <c r="D244" s="85"/>
@@ -12489,7 +12570,7 @@
       <c r="U244" s="2"/>
       <c r="AC244" s="84"/>
     </row>
-    <row r="245" spans="2:29" ht="15.75">
+    <row r="245" spans="2:29" ht="16">
       <c r="B245" s="102"/>
       <c r="C245" s="103"/>
       <c r="D245" s="85"/>
@@ -12499,7 +12580,7 @@
       <c r="U245" s="2"/>
       <c r="AC245" s="84"/>
     </row>
-    <row r="246" spans="2:29" ht="15.75">
+    <row r="246" spans="2:29" ht="16">
       <c r="B246" s="102"/>
       <c r="C246" s="103"/>
       <c r="D246" s="85"/>
@@ -12509,7 +12590,7 @@
       <c r="U246" s="2"/>
       <c r="AC246" s="84"/>
     </row>
-    <row r="247" spans="2:29" ht="15.75">
+    <row r="247" spans="2:29" ht="16">
       <c r="B247" s="102"/>
       <c r="C247" s="103"/>
       <c r="D247" s="85"/>
@@ -12519,7 +12600,7 @@
       <c r="U247" s="2"/>
       <c r="AC247" s="84"/>
     </row>
-    <row r="248" spans="2:29" ht="15.75">
+    <row r="248" spans="2:29" ht="16">
       <c r="B248" s="102"/>
       <c r="C248" s="103"/>
       <c r="D248" s="85"/>
@@ -12529,7 +12610,7 @@
       <c r="U248" s="2"/>
       <c r="AC248" s="84"/>
     </row>
-    <row r="249" spans="2:29" ht="15.75">
+    <row r="249" spans="2:29" ht="16">
       <c r="B249" s="102"/>
       <c r="C249" s="103"/>
       <c r="D249" s="85"/>
@@ -12539,7 +12620,7 @@
       <c r="U249" s="2"/>
       <c r="AC249" s="84"/>
     </row>
-    <row r="250" spans="2:29" ht="15.75">
+    <row r="250" spans="2:29" ht="16">
       <c r="B250" s="102"/>
       <c r="C250" s="103"/>
       <c r="D250" s="85"/>
@@ -12549,7 +12630,7 @@
       <c r="U250" s="2"/>
       <c r="AC250" s="84"/>
     </row>
-    <row r="251" spans="2:29" ht="15.75">
+    <row r="251" spans="2:29" ht="16">
       <c r="B251" s="102"/>
       <c r="C251" s="103"/>
       <c r="D251" s="85"/>
@@ -12559,7 +12640,7 @@
       <c r="U251" s="2"/>
       <c r="AC251" s="84"/>
     </row>
-    <row r="252" spans="2:29" ht="15.75">
+    <row r="252" spans="2:29" ht="16">
       <c r="B252" s="102"/>
       <c r="C252" s="103"/>
       <c r="D252" s="85"/>
@@ -12570,7 +12651,7 @@
       <c r="U252" s="2"/>
       <c r="AC252" s="84"/>
     </row>
-    <row r="253" spans="2:29" ht="15.75">
+    <row r="253" spans="2:29" ht="16">
       <c r="B253" s="102"/>
       <c r="C253" s="103"/>
       <c r="D253" s="85"/>
@@ -12613,11 +12694,11 @@
       <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="117" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -12736,7 +12817,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="48">
+    <row r="20" spans="1:3" ht="43.5">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -12930,7 +13011,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="48">
+    <row r="45" spans="1:3" ht="43.5">
       <c r="A45" t="s">
         <v>487</v>
       </c>
@@ -12954,7 +13035,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="48">
+    <row r="49" spans="1:3" ht="43.5">
       <c r="A49" t="s">
         <v>490</v>
       </c>
@@ -12962,7 +13043,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="48">
+    <row r="50" spans="1:3" ht="43.5">
       <c r="A50" t="s">
         <v>491</v>
       </c>
@@ -12970,7 +13051,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="48">
+    <row r="51" spans="1:3" ht="43.5">
       <c r="A51" t="s">
         <v>492</v>
       </c>
@@ -12997,7 +13078,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.95">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>501</v>
       </c>
@@ -13022,23 +13103,23 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="29.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="29.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="45.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="45.42578125" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="29.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="29.453125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="45.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.453125" style="2" customWidth="1"/>
+    <col min="13" max="14" width="45.453125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="56" customFormat="1" ht="32.1">
+    <row r="1" spans="1:14" s="56" customFormat="1" ht="29">
       <c r="A1" s="3" t="s">
         <v>325</v>
       </c>
@@ -13114,28 +13195,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.453125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.81640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="30.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="17" customWidth="1"/>
-    <col min="16" max="16" width="43.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="2"/>
+    <col min="13" max="13" width="30.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="14.453125" style="17" customWidth="1"/>
+    <col min="16" max="16" width="43.453125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="56" customFormat="1" ht="32.1">
+    <row r="1" spans="1:17" s="56" customFormat="1" ht="29">
       <c r="A1" s="10" t="s">
         <v>582</v>
       </c>
@@ -13221,25 +13302,25 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="17" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="17" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="32.85546875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="17" customWidth="1"/>
-    <col min="12" max="12" width="40.42578125" style="17" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="17" customWidth="1"/>
-    <col min="14" max="16384" width="8.85546875" style="17"/>
+    <col min="7" max="7" width="20.453125" style="17" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" style="17" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="32.81640625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="17" customWidth="1"/>
+    <col min="12" max="12" width="40.453125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="22.1796875" style="17" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="57" customFormat="1" ht="32.1">
+    <row r="1" spans="1:13" s="57" customFormat="1" ht="29">
       <c r="A1" s="60" t="s">
         <v>589</v>
       </c>
@@ -13309,31 +13390,31 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" style="58" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="55.453125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="35.453125" style="58" customWidth="1"/>
     <col min="4" max="4" width="15" style="2" customWidth="1"/>
-    <col min="5" max="6" width="29.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="58" customWidth="1"/>
+    <col min="5" max="6" width="29.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" style="58" customWidth="1"/>
     <col min="8" max="8" width="13" style="58" customWidth="1"/>
-    <col min="9" max="9" width="55.42578125" style="58" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" style="58" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="23.42578125" style="59" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="55.453125" style="58" customWidth="1"/>
+    <col min="10" max="10" width="35.453125" style="58" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.453125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="35.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.453125" style="59" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="56" customFormat="1" ht="32.1">
+    <row r="1" spans="1:14" s="56" customFormat="1" ht="29">
       <c r="A1" s="78" t="s">
         <v>595</v>
       </c>
@@ -13404,12 +13485,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee7d25ce-443e-4f8a-a748-4259b6f1626e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="129c8279-1928-4e9e-bf04-a22cc9c6a884" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13642,24 +13725,48 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee7d25ce-443e-4f8a-a748-4259b6f1626e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="129c8279-1928-4e9e-bf04-a22cc9c6a884" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B6F3CE9-A837-46EA-9FB3-9103F3863ECD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA070F5E-46B8-4CF5-94C0-070A58B7172E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee7d25ce-443e-4f8a-a748-4259b6f1626e"/>
+    <ds:schemaRef ds:uri="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80AF805D-BBAB-438F-A2B3-36BD6E56A636}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80AF805D-BBAB-438F-A2B3-36BD6E56A636}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
+    <ds:schemaRef ds:uri="ee7d25ce-443e-4f8a-a748-4259b6f1626e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA070F5E-46B8-4CF5-94C0-070A58B7172E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B6F3CE9-A837-46EA-9FB3-9103F3863ECD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>